<commit_message>
Scan for Plans and Report Definitions working
</commit_message>
<xml_diff>
--- a/GUI/Testing/SABR Plan Evaluation Worksheet BLANK For testing.xlsx
+++ b/GUI/Testing/SABR Plan Evaluation Worksheet BLANK For testing.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg\OneDrive - Queen's University\Python\Projects\EclipseRelated\PlanEvaluation\GUI\Testing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_B9C4EF12A396D4B7033C52154DBEC399ECC58F9A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16770" yWindow="-30" windowWidth="10065" windowHeight="11790" tabRatio="893" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="893" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EvaluationSheet 48Gy4F 60Gy5F" sheetId="16" r:id="rId1"/>
@@ -21,7 +27,15 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'EvaluationSheet 54Gy 3F'!$B$2:$L$52</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'EvaluationSheet 60Gy 8F'!$B$2:$L$53</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2094,7 +2108,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -3815,10 +3829,10 @@
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="3"/>
-    <cellStyle name="Percent 3" xfId="4"/>
+    <cellStyle name="Percent 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Percent 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -4005,7 +4019,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4227,6 +4241,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-97BA-4C78-8F14-D76C7A326420}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4396,6 +4415,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-97BA-4C78-8F14-D76C7A326420}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4704,7 +4728,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12316" name="Chart 2"/>
+        <xdr:cNvPr id="12316" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001C300000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -4741,7 +4771,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7341" name="Picture 1"/>
+        <xdr:cNvPr id="7341" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-0000AD1C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -4840,7 +4876,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4873,9 +4909,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4908,6 +4961,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5083,14 +5153,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet9">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P63"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7125,14 +7195,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet11">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8902,14 +8972,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet12">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10549,7 +10619,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="C1:Q43"/>
   <sheetViews>
@@ -11558,7 +11628,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="C1:Q46"/>
   <sheetViews>
@@ -12566,7 +12636,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="C1:Q43"/>
   <sheetViews>
@@ -13574,7 +13644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="H2:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Added match window working except that right click does not activate the item underneath it
</commit_message>
<xml_diff>
--- a/GUI/Testing/SABR Plan Evaluation Worksheet BLANK For testing.xlsx
+++ b/GUI/Testing/SABR Plan Evaluation Worksheet BLANK For testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg\OneDrive - Queen's University\Python\Projects\EclipseRelated\PlanEvaluation\gui\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="11_B9C4EF12A396D4B7033C52154DBEC399ECC58F9A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{73CEA0A6-064C-470F-AD11-3D8A2D2CCD2F}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="11_B9C4EF12A396D4B7033C52154DBEC399ECC58F9A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CA14E81A-455F-4F7B-ABC5-58EB8A51C346}"/>
   <bookViews>
-    <workbookView xWindow="17010" yWindow="3690" windowWidth="6990" windowHeight="9360" tabRatio="893" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9480" tabRatio="893" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EvaluationSheet 48Gy4F 60Gy5F" sheetId="16" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="217">
   <si>
     <t>Patient:</t>
   </si>
@@ -2109,6 +2109,12 @@
   </si>
   <si>
     <t>LUNR</t>
+  </si>
+  <si>
+    <t>AA, BB</t>
+  </si>
+  <si>
+    <t>LUNL</t>
   </si>
 </sst>
 </file>
@@ -2973,7 +2979,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="345">
+  <cellXfs count="353">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3475,10 +3481,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3794,6 +3796,81 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3808,78 +3885,39 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="10" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -5235,28 +5273,28 @@
     <col min="11" max="11" width="14.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="18.140625" style="1" customWidth="1"/>
     <col min="13" max="13" width="14" style="2" customWidth="1"/>
-    <col min="15" max="15" width="38.85546875" style="315" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" style="316" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.85546875" style="314" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="315" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="206" t="s">
+      <c r="B1" s="205" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="207"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="208"/>
-      <c r="G1" s="208"/>
-      <c r="H1" s="209" t="s">
+      <c r="C1" s="206"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="206"/>
+      <c r="F1" s="207"/>
+      <c r="G1" s="207"/>
+      <c r="H1" s="208" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="206"/>
-      <c r="J1" s="206"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
+      <c r="I1" s="205"/>
+      <c r="J1" s="205"/>
+      <c r="K1" s="209"/>
+      <c r="L1" s="209"/>
       <c r="M1" s="87"/>
-      <c r="O1" s="302"/>
+      <c r="O1" s="301"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="82"/>
@@ -5273,7 +5311,7 @@
       <c r="K2" s="84"/>
       <c r="L2" s="86"/>
       <c r="M2" s="87"/>
-      <c r="O2" s="302"/>
+      <c r="O2" s="301"/>
     </row>
     <row r="3" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="89"/>
@@ -5290,7 +5328,7 @@
       <c r="K3" s="91"/>
       <c r="L3" s="93"/>
       <c r="M3" s="87"/>
-      <c r="O3" s="302"/>
+      <c r="O3" s="301"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="94"/>
@@ -5317,11 +5355,11 @@
         <v>68</v>
       </c>
       <c r="M4" s="87"/>
-      <c r="O4" s="303" t="str">
+      <c r="O4" s="302" t="str">
         <f>C4</f>
         <v>Patient:</v>
       </c>
-      <c r="P4" s="308" t="str">
+      <c r="P4" s="307" t="str">
         <f>D4</f>
         <v>??</v>
       </c>
@@ -5351,11 +5389,11 @@
         <v>68</v>
       </c>
       <c r="M5" s="87"/>
-      <c r="O5" s="303" t="str">
+      <c r="O5" s="302" t="str">
         <f>C5</f>
         <v>CR#:</v>
       </c>
-      <c r="P5" s="317" t="str">
+      <c r="P5" s="316" t="str">
         <f>D5</f>
         <v>??</v>
       </c>
@@ -5375,11 +5413,11 @@
       <c r="K6" s="84"/>
       <c r="L6" s="86"/>
       <c r="M6" s="87"/>
-      <c r="O6" s="303" t="str">
+      <c r="O6" s="302" t="str">
         <f>K4</f>
         <v>Site:</v>
       </c>
-      <c r="P6" s="308" t="str">
+      <c r="P6" s="307" t="str">
         <f>L4</f>
         <v>??</v>
       </c>
@@ -5401,11 +5439,11 @@
       <c r="K7" s="97"/>
       <c r="L7" s="100"/>
       <c r="M7" s="87"/>
-      <c r="O7" s="303" t="str">
+      <c r="O7" s="302" t="str">
         <f>K5</f>
         <v>Plan Name:</v>
       </c>
-      <c r="P7" s="308" t="str">
+      <c r="P7" s="307" t="str">
         <f>L5</f>
         <v>??</v>
       </c>
@@ -5427,11 +5465,11 @@
       <c r="K8" s="97"/>
       <c r="L8" s="100"/>
       <c r="M8" s="87"/>
-      <c r="O8" s="303" t="str">
+      <c r="O8" s="302" t="str">
         <f>F4</f>
         <v>Prescription Dose (cGy):</v>
       </c>
-      <c r="P8" s="308" t="str">
+      <c r="P8" s="307" t="str">
         <f>H4</f>
         <v>??</v>
       </c>
@@ -5453,11 +5491,11 @@
       <c r="K9" s="97"/>
       <c r="L9" s="100"/>
       <c r="M9" s="87"/>
-      <c r="O9" s="303" t="str">
+      <c r="O9" s="302" t="str">
         <f>F5</f>
         <v>Fractions:</v>
       </c>
-      <c r="P9" s="308" t="str">
+      <c r="P9" s="307" t="str">
         <f>H5</f>
         <v>??</v>
       </c>
@@ -5479,11 +5517,11 @@
       <c r="K10" s="91"/>
       <c r="L10" s="93"/>
       <c r="M10" s="87"/>
-      <c r="O10" s="303" t="str">
+      <c r="O10" s="302" t="str">
         <f>C7</f>
         <v>GTV Volume (cc)</v>
       </c>
-      <c r="P10" s="308" t="str">
+      <c r="P10" s="307" t="str">
         <f>G7</f>
         <v>??</v>
       </c>
@@ -5494,28 +5532,28 @@
       </c>
       <c r="C11" s="83"/>
       <c r="D11" s="83"/>
-      <c r="E11" s="211" t="s">
+      <c r="E11" s="210" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="212"/>
-      <c r="G11" s="213"/>
-      <c r="H11" s="212"/>
+      <c r="F11" s="211"/>
+      <c r="G11" s="212"/>
+      <c r="H11" s="211"/>
       <c r="I11" s="117" t="s">
         <v>37</v>
       </c>
       <c r="J11" s="83"/>
-      <c r="K11" s="214" t="s">
+      <c r="K11" s="213" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="215" t="s">
+      <c r="L11" s="214" t="s">
         <v>37</v>
       </c>
       <c r="M11" s="87"/>
-      <c r="O11" s="303" t="str">
+      <c r="O11" s="302" t="str">
         <f>C8</f>
         <v>ITV Volume (cc):</v>
       </c>
-      <c r="P11" s="309" t="str">
+      <c r="P11" s="308" t="str">
         <f>G8</f>
         <v>??</v>
       </c>
@@ -5543,11 +5581,11 @@
       <c r="M12" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="O12" s="303" t="str">
+      <c r="O12" s="302" t="str">
         <f>C9</f>
         <v>PTV Volume (cc)</v>
       </c>
-      <c r="P12" s="310" t="str">
+      <c r="P12" s="309" t="str">
         <f>G9</f>
         <v>??</v>
       </c>
@@ -5561,19 +5599,19 @@
       <c r="G13" s="114" t="s">
         <v>184</v>
       </c>
-      <c r="H13" s="216"/>
-      <c r="I13" s="217"/>
+      <c r="H13" s="215"/>
+      <c r="I13" s="216"/>
       <c r="J13" s="96"/>
       <c r="K13" s="114" t="s">
         <v>18</v>
       </c>
       <c r="L13" s="100"/>
       <c r="M13" s="87"/>
-      <c r="O13" s="303" t="str">
+      <c r="O13" s="302" t="str">
         <f>C10</f>
         <v>Total Lung Volume (cc)</v>
       </c>
-      <c r="P13" s="309" t="str">
+      <c r="P13" s="308" t="str">
         <f>G10</f>
         <v>??</v>
       </c>
@@ -5592,7 +5630,7 @@
       <c r="H14" s="97"/>
       <c r="I14" s="96"/>
       <c r="J14" s="107"/>
-      <c r="K14" s="218" t="s">
+      <c r="K14" s="217" t="s">
         <v>165</v>
       </c>
       <c r="L14" s="10" t="str">
@@ -5602,11 +5640,11 @@
       <c r="M14" s="140" t="s">
         <v>193</v>
       </c>
-      <c r="O14" s="303" t="str">
+      <c r="O14" s="302" t="str">
         <f>C14</f>
         <v>Plan Normalization Value (%)</v>
       </c>
-      <c r="P14" s="311" t="str">
+      <c r="P14" s="310" t="str">
         <f>G14</f>
         <v>??</v>
       </c>
@@ -5622,8 +5660,8 @@
       <c r="G15" s="198" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="219"/>
-      <c r="I15" s="220"/>
+      <c r="H15" s="218"/>
+      <c r="I15" s="219"/>
       <c r="J15" s="107" t="s">
         <v>37</v>
       </c>
@@ -5637,11 +5675,11 @@
       <c r="M15" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="O15" s="303" t="str">
+      <c r="O15" s="302" t="str">
         <f>C15</f>
         <v>Dose @COM-PTV (%)</v>
       </c>
-      <c r="P15" s="311" t="str">
+      <c r="P15" s="310" t="str">
         <f>G15</f>
         <v>??</v>
       </c>
@@ -5654,18 +5692,18 @@
       <c r="D16" s="83"/>
       <c r="E16" s="83"/>
       <c r="F16" s="118"/>
-      <c r="G16" s="221"/>
+      <c r="G16" s="220"/>
       <c r="H16" s="84"/>
-      <c r="I16" s="222"/>
+      <c r="I16" s="221"/>
       <c r="J16" s="83"/>
       <c r="K16" s="119"/>
       <c r="L16" s="11"/>
       <c r="M16" s="87"/>
-      <c r="O16" s="303" t="str">
+      <c r="O16" s="302" t="str">
         <f>C17</f>
         <v>PTV- Minimum Dose (%)</v>
       </c>
-      <c r="P16" s="309" t="str">
+      <c r="P16" s="308" t="str">
         <f>G17</f>
         <v>??</v>
       </c>
@@ -5681,8 +5719,8 @@
       <c r="G17" s="198" t="s">
         <v>68</v>
       </c>
-      <c r="H17" s="223"/>
-      <c r="I17" s="220"/>
+      <c r="H17" s="222"/>
+      <c r="I17" s="219"/>
       <c r="J17" s="107"/>
       <c r="K17" s="116" t="s">
         <v>165</v>
@@ -5692,11 +5730,11 @@
         <v>??</v>
       </c>
       <c r="M17" s="87"/>
-      <c r="O17" s="303" t="str">
+      <c r="O17" s="302" t="str">
         <f>C18</f>
         <v>PTV - V100(%)</v>
       </c>
-      <c r="P17" s="309" t="str">
+      <c r="P17" s="308" t="str">
         <f>G18</f>
         <v>??</v>
       </c>
@@ -5712,7 +5750,7 @@
       <c r="G18" s="197" t="s">
         <v>68</v>
       </c>
-      <c r="H18" s="223"/>
+      <c r="H18" s="222"/>
       <c r="I18" s="122"/>
       <c r="J18" s="122"/>
       <c r="K18" s="123">
@@ -5725,11 +5763,11 @@
       <c r="M18" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="O18" s="303" t="str">
+      <c r="O18" s="302" t="str">
         <f>C19</f>
         <v>PTV - V90 (%)</v>
       </c>
-      <c r="P18" s="309" t="str">
+      <c r="P18" s="308" t="str">
         <f>G19</f>
         <v>??</v>
       </c>
@@ -5745,7 +5783,7 @@
       <c r="G19" s="196" t="s">
         <v>68</v>
       </c>
-      <c r="H19" s="224"/>
+      <c r="H19" s="223"/>
       <c r="I19" s="126"/>
       <c r="J19" s="90"/>
       <c r="K19" s="127">
@@ -5758,11 +5796,11 @@
       <c r="M19" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="O19" s="303" t="str">
+      <c r="O19" s="302" t="str">
         <f>CONCATENATE(C21," ",D21)</f>
         <v>Location V105% - PTV (cc) =</v>
       </c>
-      <c r="P19" s="312" t="str">
+      <c r="P19" s="311" t="str">
         <f>G21</f>
         <v>??</v>
       </c>
@@ -5782,11 +5820,11 @@
       <c r="K20" s="129"/>
       <c r="L20" s="14"/>
       <c r="M20" s="87"/>
-      <c r="O20" s="303" t="str">
+      <c r="O20" s="302" t="str">
         <f>CONCATENATE(C22," ",D22)</f>
         <v>Volume V100% (cc) =</v>
       </c>
-      <c r="P20" s="312" t="str">
+      <c r="P20" s="311" t="str">
         <f>G22</f>
         <v>??</v>
       </c>
@@ -5806,7 +5844,7 @@
       <c r="G21" s="194" t="s">
         <v>68</v>
       </c>
-      <c r="H21" s="225" t="str">
+      <c r="H21" s="224" t="str">
         <f>IFERROR(G21/G9,"??")</f>
         <v>??</v>
       </c>
@@ -5822,11 +5860,11 @@
       <c r="M21" s="140" t="s">
         <v>190</v>
       </c>
-      <c r="O21" s="303" t="str">
+      <c r="O21" s="302" t="str">
         <f>CONCATENATE(C24," ",D24)</f>
         <v>Location D³2cm (%) =</v>
       </c>
-      <c r="P21" s="313" t="str">
+      <c r="P21" s="312" t="str">
         <f>G24</f>
         <v>??</v>
       </c>
@@ -5864,11 +5902,11 @@
       <c r="M22" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="O22" s="303" t="str">
+      <c r="O22" s="302" t="str">
         <f>C25</f>
         <v>Volume</v>
       </c>
-      <c r="P22" s="313" t="str">
+      <c r="P22" s="312" t="str">
         <f>G25</f>
         <v xml:space="preserve"> ??</v>
       </c>
@@ -5888,11 +5926,11 @@
       <c r="K23" s="119"/>
       <c r="L23" s="11"/>
       <c r="M23" s="87"/>
-      <c r="O23" s="303" t="str">
+      <c r="O23" s="302" t="str">
         <f>C29</f>
         <v>Mean Dose (contralateral lung)</v>
       </c>
-      <c r="P23" s="313" t="str">
+      <c r="P23" s="312" t="str">
         <f>G29</f>
         <v>??</v>
       </c>
@@ -5904,7 +5942,7 @@
       <c r="C24" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="226" t="s">
+      <c r="D24" s="225" t="s">
         <v>186</v>
       </c>
       <c r="E24" s="122"/>
@@ -5912,7 +5950,7 @@
       <c r="G24" s="194" t="s">
         <v>68</v>
       </c>
-      <c r="H24" s="227"/>
+      <c r="H24" s="226"/>
       <c r="I24" s="139"/>
       <c r="J24" s="122"/>
       <c r="K24" s="199" t="str">
@@ -5926,11 +5964,11 @@
       <c r="M24" s="140" t="s">
         <v>191</v>
       </c>
-      <c r="O24" s="303" t="str">
+      <c r="O24" s="302" t="str">
         <f>C30</f>
         <v>Mean Dose (Total lung)</v>
       </c>
-      <c r="P24" s="313" t="str">
+      <c r="P24" s="312" t="str">
         <f>G30</f>
         <v>??</v>
       </c>
@@ -5942,11 +5980,11 @@
       <c r="C25" s="133" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="228" t="s">
+      <c r="D25" s="227" t="s">
         <v>185</v>
       </c>
       <c r="E25" s="90"/>
-      <c r="F25" s="229"/>
+      <c r="F25" s="228"/>
       <c r="G25" s="195" t="s">
         <v>187</v>
       </c>
@@ -5969,11 +6007,11 @@
       <c r="M25" s="140" t="s">
         <v>192</v>
       </c>
-      <c r="O25" s="303" t="str">
+      <c r="O25" s="302" t="str">
         <f>C31</f>
         <v>V20 (Total Lung) in %</v>
       </c>
-      <c r="P25" s="313" t="str">
+      <c r="P25" s="312" t="str">
         <f>G31</f>
         <v>??</v>
       </c>
@@ -5999,11 +6037,11 @@
       </c>
       <c r="L26" s="145"/>
       <c r="M26" s="87"/>
-      <c r="O26" s="303" t="str">
+      <c r="O26" s="302" t="str">
         <f>CONCATENATE(C32," ",F32)</f>
         <v xml:space="preserve">Lung-Basic Function </v>
       </c>
-      <c r="P26" s="313" t="str">
+      <c r="P26" s="312" t="str">
         <f>G32</f>
         <v>??</v>
       </c>
@@ -6027,11 +6065,11 @@
       </c>
       <c r="L27" s="145"/>
       <c r="M27" s="87"/>
-      <c r="O27" s="303" t="str">
+      <c r="O27" s="302" t="str">
         <f>CONCATENATE(C33," ",F33)</f>
         <v xml:space="preserve">Lung-Pneumonitis </v>
       </c>
-      <c r="P27" s="313" t="str">
+      <c r="P27" s="312" t="str">
         <f>G33</f>
         <v>??</v>
       </c>
@@ -6053,11 +6091,11 @@
       <c r="K28" s="119"/>
       <c r="L28" s="11"/>
       <c r="M28" s="87"/>
-      <c r="O28" s="303" t="str">
+      <c r="O28" s="302" t="str">
         <f>CONCATENATE(C35," ",F35)</f>
         <v>Aorta  (max point dose)</v>
       </c>
-      <c r="P28" s="313" t="str">
+      <c r="P28" s="312" t="str">
         <f t="shared" ref="P28:P45" si="0">G35</f>
         <v>??</v>
       </c>
@@ -6081,11 +6119,11 @@
         <v>68</v>
       </c>
       <c r="M29" s="87"/>
-      <c r="O29" s="303" t="str">
+      <c r="O29" s="302" t="str">
         <f>CONCATENATE(C35," ",F36)</f>
         <v>Aorta  V40Gy=</v>
       </c>
-      <c r="P29" s="313" t="str">
+      <c r="P29" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
@@ -6109,11 +6147,11 @@
         <v>68</v>
       </c>
       <c r="M30" s="87"/>
-      <c r="O30" s="303" t="str">
+      <c r="O30" s="302" t="str">
         <f>CONCATENATE(C37," ",F37)</f>
         <v>Artery-Pulmonary (max point dose)</v>
       </c>
-      <c r="P30" s="313" t="str">
+      <c r="P30" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
@@ -6124,10 +6162,10 @@
         <v>120</v>
       </c>
       <c r="D31" s="96"/>
-      <c r="E31" s="320" t="s">
+      <c r="E31" s="338" t="s">
         <v>175</v>
       </c>
-      <c r="F31" s="321"/>
+      <c r="F31" s="339"/>
       <c r="G31" s="197" t="s">
         <v>68</v>
       </c>
@@ -6136,21 +6174,21 @@
       </c>
       <c r="I31" s="122"/>
       <c r="J31" s="122"/>
-      <c r="K31" s="204" t="s">
+      <c r="K31" s="203" t="s">
         <v>70</v>
       </c>
       <c r="L31" s="80" t="str">
         <f>'Calculations 48Gy4F_ or_ 60Gy5F'!K34</f>
         <v>??</v>
       </c>
-      <c r="M31" s="230" t="s">
+      <c r="M31" s="229" t="s">
         <v>52</v>
       </c>
-      <c r="O31" s="303" t="str">
+      <c r="O31" s="302" t="str">
         <f>CONCATENATE(C37," ",F38)</f>
         <v>Artery-Pulmonary V40Gy=</v>
       </c>
-      <c r="P31" s="313" t="str">
+      <c r="P31" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
@@ -6161,31 +6199,31 @@
         <v>66</v>
       </c>
       <c r="D32" s="96"/>
-      <c r="E32" s="320" t="s">
+      <c r="E32" s="338" t="s">
         <v>177</v>
       </c>
-      <c r="F32" s="321"/>
+      <c r="F32" s="339"/>
       <c r="G32" s="194" t="s">
         <v>68</v>
       </c>
-      <c r="H32" s="231"/>
+      <c r="H32" s="230"/>
       <c r="I32" s="122"/>
       <c r="J32" s="122"/>
-      <c r="K32" s="232">
+      <c r="K32" s="231">
         <v>1500</v>
       </c>
       <c r="L32" s="191" t="str">
         <f>IF(G32="??","??",IF(G32&lt;=K32,"Yes","No"))</f>
         <v>??</v>
       </c>
-      <c r="M32" s="233" t="s">
+      <c r="M32" s="232" t="s">
         <v>194</v>
       </c>
-      <c r="O32" s="303" t="str">
+      <c r="O32" s="302" t="str">
         <f>CONCATENATE(C39," ",F39)</f>
         <v>Spinal Canal (max point dose)</v>
       </c>
-      <c r="P32" s="313" t="str">
+      <c r="P32" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
@@ -6196,14 +6234,14 @@
         <v>67</v>
       </c>
       <c r="D33" s="96"/>
-      <c r="E33" s="322" t="s">
+      <c r="E33" s="340" t="s">
         <v>176</v>
       </c>
-      <c r="F33" s="323"/>
+      <c r="F33" s="341"/>
       <c r="G33" s="169" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="231"/>
+      <c r="H33" s="230"/>
       <c r="I33" s="96"/>
       <c r="J33" s="96"/>
       <c r="K33" s="144">
@@ -6213,14 +6251,14 @@
         <f>IF(G33="??","??",IF(G33&lt;=K33,"Yes","No"))</f>
         <v>??</v>
       </c>
-      <c r="M33" s="233" t="s">
+      <c r="M33" s="232" t="s">
         <v>194</v>
       </c>
-      <c r="O33" s="303" t="str">
+      <c r="O33" s="302" t="str">
         <f>CONCATENATE(C39," ",F40)</f>
         <v>Spinal Canal V20.8Gy=</v>
       </c>
-      <c r="P33" s="313" t="str">
+      <c r="P33" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
@@ -6242,25 +6280,25 @@
       <c r="K34" s="119"/>
       <c r="L34" s="86"/>
       <c r="M34" s="87"/>
-      <c r="O34" s="303" t="str">
+      <c r="O34" s="302" t="str">
         <f>CONCATENATE(C39," ",F41)</f>
         <v>Spinal Canal V13.6Gy=</v>
       </c>
-      <c r="P34" s="313" t="str">
+      <c r="P34" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B35" s="94"/>
-      <c r="C35" s="205" t="s">
+      <c r="C35" s="204" t="s">
         <v>132</v>
       </c>
       <c r="D35" s="107" t="s">
         <v>37</v>
       </c>
       <c r="E35" s="122"/>
-      <c r="F35" s="234" t="s">
+      <c r="F35" s="233" t="s">
         <v>62</v>
       </c>
       <c r="G35" s="3" t="s">
@@ -6279,23 +6317,23 @@
       <c r="M35" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="O35" s="303" t="str">
+      <c r="O35" s="302" t="str">
         <f>CONCATENATE(C42," ",F42)</f>
         <v>Spinal Canal-PRV 5mm (max point dose)</v>
       </c>
-      <c r="P35" s="313" t="str">
+      <c r="P35" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
     </row>
     <row r="36" spans="2:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B36" s="94"/>
-      <c r="C36" s="235"/>
-      <c r="D36" s="236" t="s">
+      <c r="C36" s="234"/>
+      <c r="D36" s="235" t="s">
         <v>199</v>
       </c>
       <c r="E36" s="147"/>
-      <c r="F36" s="237" t="s">
+      <c r="F36" s="236" t="s">
         <v>139</v>
       </c>
       <c r="G36" s="4" t="str">
@@ -6307,7 +6345,7 @@
       </c>
       <c r="I36" s="122"/>
       <c r="J36" s="122"/>
-      <c r="K36" s="238">
+      <c r="K36" s="237">
         <v>10</v>
       </c>
       <c r="L36" s="12" t="str">
@@ -6317,11 +6355,11 @@
       <c r="M36" s="87" t="s">
         <v>167</v>
       </c>
-      <c r="O36" s="303" t="str">
+      <c r="O36" s="302" t="str">
         <f>CONCATENATE(C43," ",F43)</f>
         <v>Ipsilat. Brach. Plex. (max point dose)</v>
       </c>
-      <c r="P36" s="313" t="str">
+      <c r="P36" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
@@ -6332,8 +6370,8 @@
         <v>170</v>
       </c>
       <c r="D37" s="96"/>
-      <c r="E37" s="239"/>
-      <c r="F37" s="234" t="s">
+      <c r="E37" s="238"/>
+      <c r="F37" s="233" t="s">
         <v>62</v>
       </c>
       <c r="G37" s="4" t="s">
@@ -6344,7 +6382,7 @@
       </c>
       <c r="I37" s="122"/>
       <c r="J37" s="122"/>
-      <c r="K37" s="238">
+      <c r="K37" s="237">
         <v>4800</v>
       </c>
       <c r="L37" s="12" t="str">
@@ -6354,23 +6392,23 @@
       <c r="M37" s="87" t="s">
         <v>167</v>
       </c>
-      <c r="O37" s="303" t="str">
+      <c r="O37" s="302" t="str">
         <f>CONCATENATE(C43," ",F44)</f>
         <v>Ipsilat. Brach. Plex. V23.6Gy=</v>
       </c>
-      <c r="P37" s="313" t="str">
+      <c r="P37" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
     </row>
     <row r="38" spans="2:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B38" s="94"/>
-      <c r="C38" s="235"/>
-      <c r="D38" s="236" t="s">
+      <c r="C38" s="234"/>
+      <c r="D38" s="235" t="s">
         <v>199</v>
       </c>
       <c r="E38" s="147"/>
-      <c r="F38" s="237" t="s">
+      <c r="F38" s="236" t="s">
         <v>139</v>
       </c>
       <c r="G38" s="4" t="str">
@@ -6380,7 +6418,7 @@
       <c r="H38" s="131"/>
       <c r="I38" s="122"/>
       <c r="J38" s="122"/>
-      <c r="K38" s="238">
+      <c r="K38" s="237">
         <v>10</v>
       </c>
       <c r="L38" s="12" t="str">
@@ -6390,11 +6428,11 @@
       <c r="M38" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="O38" s="303" t="str">
+      <c r="O38" s="302" t="str">
         <f>CONCATENATE(C45," ",F45)</f>
         <v>Skin V30Gy=</v>
       </c>
-      <c r="P38" s="313" t="str">
+      <c r="P38" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
@@ -6406,7 +6444,7 @@
       </c>
       <c r="D39" s="96"/>
       <c r="E39" s="122"/>
-      <c r="F39" s="240" t="s">
+      <c r="F39" s="239" t="s">
         <v>62</v>
       </c>
       <c r="G39" s="169" t="s">
@@ -6427,11 +6465,11 @@
       <c r="M39" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="O39" s="303" t="str">
+      <c r="O39" s="302" t="str">
         <f>CONCATENATE(C46," ",F46)</f>
         <v>Heart (max point dose)</v>
       </c>
-      <c r="P39" s="313" t="str">
+      <c r="P39" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
@@ -6439,11 +6477,11 @@
     <row r="40" spans="2:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B40" s="94"/>
       <c r="C40" s="94"/>
-      <c r="D40" s="324" t="s">
+      <c r="D40" s="342" t="s">
         <v>196</v>
       </c>
-      <c r="E40" s="325"/>
-      <c r="F40" s="241" t="s">
+      <c r="E40" s="343"/>
+      <c r="F40" s="240" t="s">
         <v>146</v>
       </c>
       <c r="G40" s="4" t="str">
@@ -6463,11 +6501,11 @@
       <c r="M40" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="O40" s="303" t="str">
+      <c r="O40" s="302" t="str">
         <f>CONCATENATE(C46," ",F47)</f>
         <v>Heart V28Gy=</v>
       </c>
-      <c r="P40" s="313" t="str">
+      <c r="P40" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
@@ -6479,7 +6517,7 @@
         <v>198</v>
       </c>
       <c r="E41" s="147"/>
-      <c r="F41" s="242" t="s">
+      <c r="F41" s="241" t="s">
         <v>147</v>
       </c>
       <c r="G41" s="4" t="str">
@@ -6499,23 +6537,23 @@
       <c r="M41" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="O41" s="303" t="str">
+      <c r="O41" s="302" t="str">
         <f>CONCATENATE(C48," ",F48)</f>
         <v>Esophagus (max point dose)</v>
       </c>
-      <c r="P41" s="313" t="str">
+      <c r="P41" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B42" s="94"/>
-      <c r="C42" s="243" t="s">
+      <c r="C42" s="242" t="s">
         <v>35</v>
       </c>
       <c r="D42" s="122"/>
       <c r="E42" s="122"/>
-      <c r="F42" s="244" t="s">
+      <c r="F42" s="243" t="s">
         <v>62</v>
       </c>
       <c r="G42" s="194" t="s">
@@ -6532,23 +6570,23 @@
         <v>??</v>
       </c>
       <c r="M42" s="87"/>
-      <c r="O42" s="303" t="str">
+      <c r="O42" s="302" t="str">
         <f>CONCATENATE(C48," ",F49)</f>
         <v>Esophagus V18.8Gy=</v>
       </c>
-      <c r="P42" s="313" t="str">
+      <c r="P42" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B43" s="94"/>
-      <c r="C43" s="205" t="s">
+      <c r="C43" s="204" t="s">
         <v>189</v>
       </c>
       <c r="D43" s="107"/>
       <c r="E43" s="122"/>
-      <c r="F43" s="234" t="s">
+      <c r="F43" s="233" t="s">
         <v>62</v>
       </c>
       <c r="G43" s="170" t="s">
@@ -6567,11 +6605,11 @@
       <c r="M43" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="O43" s="303" t="str">
+      <c r="O43" s="302" t="str">
         <f>CONCATENATE(C50," ",F50)</f>
         <v>*Chestwall (rib) (max point dose)</v>
       </c>
-      <c r="P43" s="313" t="str">
+      <c r="P43" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
@@ -6585,7 +6623,7 @@
       <c r="E44" s="152" t="s">
         <v>37</v>
       </c>
-      <c r="F44" s="242" t="s">
+      <c r="F44" s="241" t="s">
         <v>148</v>
       </c>
       <c r="G44" s="4" t="str">
@@ -6605,25 +6643,25 @@
       <c r="M44" s="140" t="s">
         <v>195</v>
       </c>
-      <c r="O44" s="303" t="str">
+      <c r="O44" s="302" t="str">
         <f>CONCATENATE(C50," ",F51)</f>
         <v>*Chestwall (rib) V40Gy=</v>
       </c>
-      <c r="P44" s="313" t="str">
+      <c r="P44" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
     </row>
     <row r="45" spans="2:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B45" s="94"/>
-      <c r="C45" s="243" t="s">
+      <c r="C45" s="242" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="226" t="s">
+      <c r="D45" s="225" t="s">
         <v>201</v>
       </c>
       <c r="E45" s="122"/>
-      <c r="F45" s="241" t="s">
+      <c r="F45" s="240" t="s">
         <v>121</v>
       </c>
       <c r="G45" s="194" t="s">
@@ -6644,11 +6682,11 @@
       <c r="M45" s="140" t="s">
         <v>195</v>
       </c>
-      <c r="O45" s="303" t="str">
+      <c r="O45" s="302" t="str">
         <f>CONCATENATE(C50," ",F52)</f>
         <v>*Chestwall (rib) V30Gy=</v>
       </c>
-      <c r="P45" s="313" t="str">
+      <c r="P45" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
@@ -6660,7 +6698,7 @@
       </c>
       <c r="D46" s="107"/>
       <c r="E46" s="122"/>
-      <c r="F46" s="240" t="s">
+      <c r="F46" s="239" t="s">
         <v>62</v>
       </c>
       <c r="G46" s="170" t="s">
@@ -6679,25 +6717,25 @@
       <c r="M46" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="O46" s="303" t="str">
+      <c r="O46" s="302" t="str">
         <f>CONCATENATE(A53," ",F53)</f>
         <v>Trachea (max point dose)</v>
       </c>
-      <c r="P46" s="314">
+      <c r="P46" s="313">
         <f>A54</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B47" s="94"/>
-      <c r="C47" s="235" t="s">
+      <c r="C47" s="234" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="236" t="s">
+      <c r="D47" s="235" t="s">
         <v>202</v>
       </c>
       <c r="E47" s="147"/>
-      <c r="F47" s="245" t="s">
+      <c r="F47" s="244" t="s">
         <v>122</v>
       </c>
       <c r="G47" s="4" t="str">
@@ -6717,11 +6755,11 @@
       <c r="M47" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="O47" s="303" t="str">
+      <c r="O47" s="302" t="str">
         <f>CONCATENATE(A53," ",F55)</f>
         <v>Trachea V15.6Gy=</v>
       </c>
-      <c r="P47" s="314">
+      <c r="P47" s="313">
         <f>A55</f>
         <v>0</v>
       </c>
@@ -6733,7 +6771,7 @@
       </c>
       <c r="D48" s="96"/>
       <c r="E48" s="122"/>
-      <c r="F48" s="240" t="s">
+      <c r="F48" s="239" t="s">
         <v>62</v>
       </c>
       <c r="G48" s="170" t="s">
@@ -6752,11 +6790,11 @@
       <c r="M48" s="140" t="s">
         <v>195</v>
       </c>
-      <c r="O48" s="303" t="str">
+      <c r="O48" s="302" t="str">
         <f>CONCATENATE(B53," ",F53)</f>
         <v>Bronchus (max point dose)</v>
       </c>
-      <c r="P48" s="314">
+      <c r="P48" s="313">
         <f>B54</f>
         <v>0</v>
       </c>
@@ -6764,11 +6802,11 @@
     <row r="49" spans="1:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B49" s="94"/>
       <c r="C49" s="177"/>
-      <c r="D49" s="246" t="s">
+      <c r="D49" s="245" t="s">
         <v>203</v>
       </c>
       <c r="E49" s="147"/>
-      <c r="F49" s="245" t="s">
+      <c r="F49" s="244" t="s">
         <v>123</v>
       </c>
       <c r="G49" s="4" t="str">
@@ -6786,11 +6824,11 @@
         <v>??</v>
       </c>
       <c r="M49" s="87"/>
-      <c r="O49" s="303" t="str">
+      <c r="O49" s="302" t="str">
         <f>CONCATENATE(B53," ",F55)</f>
         <v>Bronchus V15.6Gy=</v>
       </c>
-      <c r="P49" s="314">
+      <c r="P49" s="313">
         <f>B55</f>
         <v>0</v>
       </c>
@@ -6802,7 +6840,7 @@
       </c>
       <c r="D50" s="107"/>
       <c r="E50" s="122"/>
-      <c r="F50" s="240" t="s">
+      <c r="F50" s="239" t="s">
         <v>62</v>
       </c>
       <c r="G50" s="170" t="s">
@@ -6821,11 +6859,11 @@
       <c r="M50" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="O50" s="303" t="str">
+      <c r="O50" s="302" t="str">
         <f>CONCATENATE(C53," ",C54," ",F53)</f>
         <v>Proximal Trachea and Bronchial Tree (max point dose)</v>
       </c>
-      <c r="P50" s="313" t="str">
+      <c r="P50" s="312" t="str">
         <f>G53</f>
         <v>??</v>
       </c>
@@ -6837,7 +6875,7 @@
         <v>204</v>
       </c>
       <c r="E51" s="96"/>
-      <c r="F51" s="242" t="s">
+      <c r="F51" s="241" t="s">
         <v>139</v>
       </c>
       <c r="G51" s="4" t="str">
@@ -6857,11 +6895,11 @@
       <c r="M51" s="87" t="s">
         <v>167</v>
       </c>
-      <c r="O51" s="303" t="str">
+      <c r="O51" s="302" t="str">
         <f>CONCATENATE(C53," ",C54," ",F55)</f>
         <v>Proximal Trachea and Bronchial Tree V15.6Gy=</v>
       </c>
-      <c r="P51" s="313" t="str">
+      <c r="P51" s="312" t="str">
         <f>G55</f>
         <v>??</v>
       </c>
@@ -6869,13 +6907,13 @@
     <row r="52" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="94"/>
       <c r="C52" s="94"/>
-      <c r="D52" s="247" t="s">
+      <c r="D52" s="246" t="s">
         <v>197</v>
       </c>
-      <c r="E52" s="248" t="s">
+      <c r="E52" s="247" t="s">
         <v>37</v>
       </c>
-      <c r="F52" s="249" t="s">
+      <c r="F52" s="248" t="s">
         <v>121</v>
       </c>
       <c r="G52" s="7" t="str">
@@ -6895,20 +6933,20 @@
       <c r="M52" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="O52" s="303" t="str">
+      <c r="O52" s="302" t="str">
         <f>CONCATENATE(C56," ",C57," ",F56)</f>
         <v>Stomach and Intestines (max point dose)</v>
       </c>
-      <c r="P52" s="313" t="str">
+      <c r="P52" s="312" t="str">
         <f>G56</f>
         <v>??</v>
       </c>
     </row>
     <row r="53" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="294" t="s">
+      <c r="A53" s="293" t="s">
         <v>209</v>
       </c>
-      <c r="B53" s="295" t="s">
+      <c r="B53" s="294" t="s">
         <v>210</v>
       </c>
       <c r="C53" s="151" t="s">
@@ -6916,7 +6954,7 @@
       </c>
       <c r="D53" s="107"/>
       <c r="E53" s="107"/>
-      <c r="F53" s="250" t="s">
+      <c r="F53" s="249" t="s">
         <v>62</v>
       </c>
       <c r="G53" s="194" t="str">
@@ -6931,27 +6969,27 @@
       <c r="K53" s="116">
         <v>3480</v>
       </c>
-      <c r="L53" s="251" t="str">
+      <c r="L53" s="250" t="str">
         <f>IF(G53="??","??",IF(G53&lt;=3480,"Yes","No"))</f>
         <v>??</v>
       </c>
       <c r="M53" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="O53" s="303" t="str">
+      <c r="O53" s="302" t="str">
         <f>CONCATENATE(C56," ",C57," ",F57)</f>
         <v>Stomach and Intestines V21Gy=</v>
       </c>
-      <c r="P53" s="313" t="str">
+      <c r="P53" s="312" t="str">
         <f>G57</f>
         <v>??</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A54" s="296">
+      <c r="A54" s="295">
         <v>0</v>
       </c>
-      <c r="B54" s="297">
+      <c r="B54" s="296">
         <v>0</v>
       </c>
       <c r="C54" s="94" t="s">
@@ -6959,7 +6997,7 @@
       </c>
       <c r="D54" s="96"/>
       <c r="E54" s="147"/>
-      <c r="F54" s="252"/>
+      <c r="F54" s="251"/>
       <c r="G54" s="171" t="s">
         <v>37</v>
       </c>
@@ -6967,30 +7005,30 @@
       <c r="I54" s="147"/>
       <c r="J54" s="147"/>
       <c r="K54" s="148"/>
-      <c r="L54" s="253"/>
+      <c r="L54" s="252"/>
       <c r="M54" s="87"/>
-      <c r="O54" s="303" t="str">
+      <c r="O54" s="302" t="str">
         <f>C58</f>
         <v>Dosimetrist:</v>
       </c>
-      <c r="P54" s="307" t="str">
+      <c r="P54" s="306" t="str">
         <f>C59</f>
         <v>??</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="298">
+      <c r="A55" s="297">
         <v>0</v>
       </c>
-      <c r="B55" s="299">
+      <c r="B55" s="298">
         <v>0</v>
       </c>
       <c r="C55" s="177"/>
-      <c r="D55" s="236" t="s">
+      <c r="D55" s="235" t="s">
         <v>205</v>
       </c>
       <c r="E55" s="147"/>
-      <c r="F55" s="245" t="s">
+      <c r="F55" s="244" t="s">
         <v>124</v>
       </c>
       <c r="G55" s="194" t="str">
@@ -7012,11 +7050,11 @@
       <c r="M55" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="O55" s="303" t="str">
+      <c r="O55" s="302" t="str">
         <f>G58</f>
         <v>Physicist:</v>
       </c>
-      <c r="P55" s="307" t="str">
+      <c r="P55" s="306" t="str">
         <f>G59</f>
         <v>??</v>
       </c>
@@ -7028,7 +7066,7 @@
       </c>
       <c r="D56" s="96"/>
       <c r="E56" s="122"/>
-      <c r="F56" s="240" t="s">
+      <c r="F56" s="239" t="s">
         <v>62</v>
       </c>
       <c r="G56" s="194" t="s">
@@ -7047,25 +7085,25 @@
       <c r="M56" s="87" t="s">
         <v>167</v>
       </c>
-      <c r="O56" s="303" t="str">
+      <c r="O56" s="302" t="str">
         <f>K58</f>
         <v>Radiation Oncologist:</v>
       </c>
-      <c r="P56" s="307" t="str">
+      <c r="P56" s="306" t="str">
         <f>K59</f>
         <v>??</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B57" s="94"/>
-      <c r="C57" s="254" t="s">
+      <c r="C57" s="253" t="s">
         <v>138</v>
       </c>
-      <c r="D57" s="255" t="s">
+      <c r="D57" s="254" t="s">
         <v>208</v>
       </c>
       <c r="E57" s="96"/>
-      <c r="F57" s="242" t="s">
+      <c r="F57" s="241" t="s">
         <v>166</v>
       </c>
       <c r="G57" s="167" t="str">
@@ -7087,11 +7125,11 @@
       <c r="M57" s="87" t="s">
         <v>167</v>
       </c>
-      <c r="O57" s="303" t="str">
+      <c r="O57" s="302" t="str">
         <f>B60</f>
         <v>NOTES:</v>
       </c>
-      <c r="P57" s="307">
+      <c r="P57" s="306">
         <f>C60</f>
         <v>0</v>
       </c>
@@ -7161,17 +7199,17 @@
       <c r="C61" s="90"/>
       <c r="D61" s="90"/>
       <c r="E61" s="90"/>
-      <c r="F61" s="256" t="s">
+      <c r="F61" s="255" t="s">
         <v>128</v>
       </c>
-      <c r="G61" s="257" t="s">
+      <c r="G61" s="256" t="s">
         <v>126</v>
       </c>
-      <c r="H61" s="256"/>
-      <c r="I61" s="257"/>
-      <c r="J61" s="257"/>
-      <c r="K61" s="256"/>
-      <c r="L61" s="258"/>
+      <c r="H61" s="255"/>
+      <c r="I61" s="256"/>
+      <c r="J61" s="256"/>
+      <c r="K61" s="255"/>
+      <c r="L61" s="257"/>
       <c r="M61" s="87"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
@@ -7258,7 +7296,7 @@
   </sheetPr>
   <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -7275,28 +7313,28 @@
     <col min="11" max="11" width="14.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" style="1" customWidth="1"/>
     <col min="13" max="13" width="14" style="2" customWidth="1"/>
-    <col min="15" max="15" width="38.85546875" style="315" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" style="316" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.85546875" style="314" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="315" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="206" t="s">
+      <c r="B1" s="205" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="207"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="208"/>
-      <c r="G1" s="208"/>
-      <c r="H1" s="209" t="s">
+      <c r="C1" s="206"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="206"/>
+      <c r="F1" s="207"/>
+      <c r="G1" s="207"/>
+      <c r="H1" s="208" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="206"/>
-      <c r="J1" s="206"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
+      <c r="I1" s="205"/>
+      <c r="J1" s="205"/>
+      <c r="K1" s="209"/>
+      <c r="L1" s="209"/>
       <c r="M1" s="87"/>
-      <c r="O1" s="302"/>
+      <c r="O1" s="301"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="82"/>
@@ -7313,7 +7351,7 @@
       <c r="K2" s="84"/>
       <c r="L2" s="86"/>
       <c r="M2" s="87"/>
-      <c r="O2" s="302"/>
+      <c r="O2" s="301"/>
     </row>
     <row r="3" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="89"/>
@@ -7330,22 +7368,22 @@
       <c r="K3" s="91"/>
       <c r="L3" s="93"/>
       <c r="M3" s="87"/>
-      <c r="O3" s="302"/>
+      <c r="O3" s="301"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="94"/>
       <c r="C4" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>68</v>
+      <c r="D4" s="319" t="s">
+        <v>215</v>
       </c>
       <c r="E4" s="96"/>
       <c r="F4" s="95" t="s">
         <v>174</v>
       </c>
       <c r="G4" s="97"/>
-      <c r="H4" s="163">
+      <c r="H4" s="324">
         <v>6000</v>
       </c>
       <c r="I4" s="96"/>
@@ -7357,13 +7395,13 @@
         <v>68</v>
       </c>
       <c r="M4" s="87"/>
-      <c r="O4" s="303" t="str">
+      <c r="O4" s="302" t="str">
         <f>C4</f>
         <v>Patient:</v>
       </c>
-      <c r="P4" s="308" t="str">
+      <c r="P4" s="307" t="str">
         <f>D4</f>
-        <v>??</v>
+        <v>AA, BB</v>
       </c>
     </row>
     <row r="5" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -7371,8 +7409,8 @@
       <c r="C5" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>68</v>
+      <c r="D5" s="20">
+        <v>11</v>
       </c>
       <c r="E5" s="96"/>
       <c r="F5" s="95" t="s">
@@ -7387,17 +7425,17 @@
       <c r="K5" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="18" t="s">
-        <v>68</v>
+      <c r="L5" s="320" t="s">
+        <v>216</v>
       </c>
       <c r="M5" s="87"/>
-      <c r="O5" s="303" t="str">
+      <c r="O5" s="302" t="str">
         <f>C5</f>
         <v>CR#:</v>
       </c>
-      <c r="P5" s="308" t="str">
+      <c r="P5" s="307">
         <f>D5</f>
-        <v>??</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
@@ -7415,11 +7453,11 @@
       <c r="K6" s="84"/>
       <c r="L6" s="86"/>
       <c r="M6" s="87"/>
-      <c r="O6" s="303" t="str">
+      <c r="O6" s="302" t="str">
         <f>K4</f>
         <v>Site:</v>
       </c>
-      <c r="P6" s="308" t="str">
+      <c r="P6" s="307" t="str">
         <f>L4</f>
         <v>??</v>
       </c>
@@ -7432,8 +7470,8 @@
       <c r="D7" s="96"/>
       <c r="E7" s="96"/>
       <c r="F7" s="97"/>
-      <c r="G7" s="175" t="s">
-        <v>68</v>
+      <c r="G7" s="321">
+        <v>12.2</v>
       </c>
       <c r="H7" s="97"/>
       <c r="I7" s="96"/>
@@ -7441,13 +7479,13 @@
       <c r="K7" s="97"/>
       <c r="L7" s="100"/>
       <c r="M7" s="87"/>
-      <c r="O7" s="303" t="str">
+      <c r="O7" s="302" t="str">
         <f>K5</f>
         <v>Plan Name:</v>
       </c>
-      <c r="P7" s="308" t="str">
+      <c r="P7" s="307" t="str">
         <f>L5</f>
-        <v>??</v>
+        <v>LUNL</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.2">
@@ -7458,8 +7496,8 @@
       <c r="D8" s="96"/>
       <c r="E8" s="96"/>
       <c r="F8" s="97"/>
-      <c r="G8" s="22" t="s">
-        <v>68</v>
+      <c r="G8" s="322">
+        <v>12.1</v>
       </c>
       <c r="H8" s="97"/>
       <c r="I8" s="96"/>
@@ -7469,11 +7507,11 @@
         <v>37</v>
       </c>
       <c r="M8" s="87"/>
-      <c r="O8" s="303" t="str">
+      <c r="O8" s="302" t="str">
         <f>F4</f>
         <v>Prescription Dose (cGy):</v>
       </c>
-      <c r="P8" s="308">
+      <c r="P8" s="307">
         <f>H4</f>
         <v>6000</v>
       </c>
@@ -7486,8 +7524,8 @@
       <c r="D9" s="96"/>
       <c r="E9" s="96"/>
       <c r="F9" s="97"/>
-      <c r="G9" s="175" t="s">
-        <v>68</v>
+      <c r="G9" s="321">
+        <v>36.799999999999997</v>
       </c>
       <c r="H9" s="97"/>
       <c r="I9" s="96"/>
@@ -7495,11 +7533,11 @@
       <c r="K9" s="97"/>
       <c r="L9" s="100"/>
       <c r="M9" s="87"/>
-      <c r="O9" s="303" t="str">
+      <c r="O9" s="302" t="str">
         <f>F5</f>
         <v>Fractions:</v>
       </c>
-      <c r="P9" s="308">
+      <c r="P9" s="307">
         <f>H5</f>
         <v>8</v>
       </c>
@@ -7512,8 +7550,8 @@
       <c r="D10" s="90"/>
       <c r="E10" s="90"/>
       <c r="F10" s="91"/>
-      <c r="G10" s="23" t="s">
-        <v>68</v>
+      <c r="G10" s="323">
+        <v>3431.8</v>
       </c>
       <c r="H10" s="91"/>
       <c r="I10" s="90"/>
@@ -7521,13 +7559,13 @@
       <c r="K10" s="91"/>
       <c r="L10" s="93"/>
       <c r="M10" s="87"/>
-      <c r="O10" s="303" t="str">
+      <c r="O10" s="302" t="str">
         <f>C7</f>
         <v>GTV Volume (cc)</v>
       </c>
-      <c r="P10" s="308" t="str">
+      <c r="P10" s="307">
         <f>G7</f>
-        <v>??</v>
+        <v>12.2</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
@@ -7553,13 +7591,13 @@
         <v>37</v>
       </c>
       <c r="M11" s="87"/>
-      <c r="O11" s="303" t="str">
+      <c r="O11" s="302" t="str">
         <f>C8</f>
         <v>ITV Volume (cc):</v>
       </c>
-      <c r="P11" s="309" t="str">
+      <c r="P11" s="308">
         <f>G8</f>
-        <v>??</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
@@ -7587,13 +7625,13 @@
       <c r="M12" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="O12" s="303" t="str">
+      <c r="O12" s="302" t="str">
         <f>C9</f>
         <v>PTV Volume (cc)</v>
       </c>
-      <c r="P12" s="310" t="str">
+      <c r="P12" s="309">
         <f>G9</f>
-        <v>??</v>
+        <v>36.799999999999997</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
@@ -7602,7 +7640,7 @@
       <c r="D13" s="96"/>
       <c r="E13" s="96"/>
       <c r="F13" s="97"/>
-      <c r="G13" s="259" t="s">
+      <c r="G13" s="258" t="s">
         <v>184</v>
       </c>
       <c r="H13" s="104"/>
@@ -7613,13 +7651,13 @@
       </c>
       <c r="L13" s="100"/>
       <c r="M13" s="87"/>
-      <c r="O13" s="303" t="str">
+      <c r="O13" s="302" t="str">
         <f>C10</f>
         <v>Total Lung Volume (cc)</v>
       </c>
-      <c r="P13" s="309" t="str">
+      <c r="P13" s="308">
         <f>G10</f>
-        <v>??</v>
+        <v>3431.8</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
@@ -7633,10 +7671,10 @@
       <c r="G14" s="200" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="260"/>
-      <c r="I14" s="220"/>
+      <c r="H14" s="259"/>
+      <c r="I14" s="219"/>
       <c r="J14" s="107"/>
-      <c r="K14" s="218" t="s">
+      <c r="K14" s="217" t="s">
         <v>165</v>
       </c>
       <c r="L14" s="10" t="str">
@@ -7646,11 +7684,11 @@
       <c r="M14" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="O14" s="303" t="str">
+      <c r="O14" s="302" t="str">
         <f>C14</f>
         <v>Plan Normalization Value (%)</v>
       </c>
-      <c r="P14" s="311" t="str">
+      <c r="P14" s="310" t="str">
         <f>G14</f>
         <v>??</v>
       </c>
@@ -7666,7 +7704,7 @@
       <c r="G15" s="198" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="219"/>
+      <c r="H15" s="218"/>
       <c r="I15" s="155"/>
       <c r="J15" s="107" t="s">
         <v>37</v>
@@ -7681,11 +7719,11 @@
       <c r="M15" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="O15" s="303" t="str">
+      <c r="O15" s="302" t="str">
         <f>C15</f>
         <v>Dose @COM-PTV (cGy)</v>
       </c>
-      <c r="P15" s="311" t="str">
+      <c r="P15" s="310" t="str">
         <f>G15</f>
         <v>??</v>
       </c>
@@ -7698,20 +7736,20 @@
       <c r="D16" s="83"/>
       <c r="E16" s="83"/>
       <c r="F16" s="118"/>
-      <c r="G16" s="221"/>
+      <c r="G16" s="220"/>
       <c r="H16" s="84"/>
       <c r="I16" s="156"/>
       <c r="J16" s="83"/>
       <c r="K16" s="119"/>
       <c r="L16" s="11"/>
       <c r="M16" s="87"/>
-      <c r="O16" s="303" t="str">
+      <c r="O16" s="302" t="str">
         <f>C17</f>
         <v>PTV- Minimum Dose</v>
       </c>
-      <c r="P16" s="309" t="str">
+      <c r="P16" s="308">
         <f>G17</f>
-        <v>??</v>
+        <v>0.8590000000000001</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
@@ -7722,10 +7760,10 @@
       <c r="D17" s="107"/>
       <c r="E17" s="107"/>
       <c r="F17" s="120"/>
-      <c r="G17" s="198" t="s">
-        <v>68</v>
-      </c>
-      <c r="H17" s="223"/>
+      <c r="G17" s="344">
+        <v>0.8590000000000001</v>
+      </c>
+      <c r="H17" s="222"/>
       <c r="I17" s="155"/>
       <c r="J17" s="107"/>
       <c r="K17" s="116" t="s">
@@ -7733,16 +7771,16 @@
       </c>
       <c r="L17" s="10" t="str">
         <f>IF(G17="??","??",IF((AND((G17&gt;=60%),(G17&lt;=95%))),"Yes", "No"))</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="M17" s="87"/>
-      <c r="O17" s="303" t="str">
+      <c r="O17" s="302" t="str">
         <f>C18</f>
         <v>PTV - V100(%)</v>
       </c>
-      <c r="P17" s="309" t="str">
+      <c r="P17" s="308">
         <f>G18</f>
-        <v>??</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -7753,10 +7791,10 @@
       <c r="D18" s="96"/>
       <c r="E18" s="96"/>
       <c r="F18" s="121"/>
-      <c r="G18" s="197" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="223"/>
+      <c r="G18" s="197">
+        <v>0.95</v>
+      </c>
+      <c r="H18" s="222"/>
       <c r="I18" s="122"/>
       <c r="J18" s="122"/>
       <c r="K18" s="123">
@@ -7764,18 +7802,18 @@
       </c>
       <c r="L18" s="192" t="str">
         <f>IF(G18="??","??",(IF(G18&gt;=95%,"Yes","No")))</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="M18" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="O18" s="303" t="str">
+      <c r="O18" s="302" t="str">
         <f>C19</f>
         <v>PTV - V90 (%)</v>
       </c>
-      <c r="P18" s="309" t="str">
+      <c r="P18" s="308">
         <f>G19</f>
-        <v>??</v>
+        <v>0.99915200000000004</v>
       </c>
     </row>
     <row r="19" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -7786,10 +7824,10 @@
       <c r="D19" s="90"/>
       <c r="E19" s="90"/>
       <c r="F19" s="125"/>
-      <c r="G19" s="196" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="224"/>
+      <c r="G19" s="196">
+        <v>0.99915200000000004</v>
+      </c>
+      <c r="H19" s="223"/>
       <c r="I19" s="126"/>
       <c r="J19" s="90"/>
       <c r="K19" s="127">
@@ -7797,18 +7835,18 @@
       </c>
       <c r="L19" s="192" t="str">
         <f>IF(G19="??","??",(IF(G19&gt;=99%,"Yes","No")))</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="M19" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="O19" s="303" t="str">
+      <c r="O19" s="302" t="str">
         <f>CONCATENATE(C21," ",D21)</f>
         <v>Location V105% - PTV (cc) =</v>
       </c>
-      <c r="P19" s="312" t="str">
+      <c r="P19" s="311">
         <f>G21</f>
-        <v>??</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.2">
@@ -7826,13 +7864,13 @@
       <c r="K20" s="129"/>
       <c r="L20" s="14"/>
       <c r="M20" s="87"/>
-      <c r="O20" s="303" t="str">
+      <c r="O20" s="302" t="str">
         <f>CONCATENATE(C22," ",D22)</f>
         <v>Volume V100% (cc) =</v>
       </c>
-      <c r="P20" s="312" t="str">
+      <c r="P20" s="311">
         <f>G22</f>
-        <v>??</v>
+        <v>38.9</v>
       </c>
     </row>
     <row r="21" spans="2:16" ht="15.75" x14ac:dyDescent="0.3">
@@ -7847,12 +7885,12 @@
       </c>
       <c r="E21" s="122"/>
       <c r="F21" s="131"/>
-      <c r="G21" s="194" t="s">
-        <v>68</v>
-      </c>
-      <c r="H21" s="172" t="str">
+      <c r="G21" s="345">
+        <v>0</v>
+      </c>
+      <c r="H21" s="172">
         <f>IFERROR(G21/G9,"??")</f>
-        <v>??</v>
+        <v>0</v>
       </c>
       <c r="I21" s="122"/>
       <c r="J21" s="122"/>
@@ -7861,18 +7899,18 @@
       </c>
       <c r="L21" s="12" t="str">
         <f>IF(G21="??","??",IF(H21&lt;15%,"Yes","No"))</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="M21" s="140" t="s">
         <v>190</v>
       </c>
-      <c r="O21" s="303" t="str">
+      <c r="O21" s="302" t="str">
         <f>CONCATENATE(C24," ",D24)</f>
         <v>Location D³2cm (%) =</v>
       </c>
-      <c r="P21" s="313" t="str">
+      <c r="P21" s="312">
         <f>G24</f>
-        <v>??</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -7889,12 +7927,12 @@
       <c r="F22" s="174" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="195" t="s">
-        <v>68</v>
-      </c>
-      <c r="H22" s="173" t="str">
+      <c r="G22" s="346">
+        <v>38.9</v>
+      </c>
+      <c r="H22" s="173">
         <f>IFERROR(G22/G9,"??")</f>
-        <v>??</v>
+        <v>1.0570652173913044</v>
       </c>
       <c r="I22" s="134" t="s">
         <v>37</v>
@@ -7904,19 +7942,19 @@
         <v>12</v>
       </c>
       <c r="L22" s="13" t="str">
-        <f>'Calculations 60Gy_8F'!K31</f>
-        <v>??</v>
+        <f ca="1">'Calculations 60Gy_8F'!K31</f>
+        <v>Yes</v>
       </c>
       <c r="M22" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="O22" s="303" t="str">
+      <c r="O22" s="302" t="str">
         <f>CONCATENATE(C25," ",D25)</f>
         <v>Volume V50% (cc) =</v>
       </c>
-      <c r="P22" s="313" t="str">
+      <c r="P22" s="312">
         <f>G25</f>
-        <v>??</v>
+        <v>161.5</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
@@ -7934,13 +7972,13 @@
       <c r="K23" s="119"/>
       <c r="L23" s="11"/>
       <c r="M23" s="87"/>
-      <c r="O23" s="303" t="str">
+      <c r="O23" s="302" t="str">
         <f>C29</f>
         <v>Mean Dose (contralateral lung)</v>
       </c>
-      <c r="P23" s="313" t="str">
+      <c r="P23" s="312">
         <f>G29</f>
-        <v>??</v>
+        <v>468</v>
       </c>
     </row>
     <row r="24" spans="2:16" ht="14.25" x14ac:dyDescent="0.25">
@@ -7955,30 +7993,30 @@
       </c>
       <c r="E24" s="122"/>
       <c r="F24" s="137"/>
-      <c r="G24" s="203" t="s">
-        <v>68</v>
+      <c r="G24" s="347">
+        <v>54</v>
       </c>
       <c r="H24" s="138"/>
       <c r="I24" s="139"/>
       <c r="J24" s="122"/>
-      <c r="K24" s="157" t="str">
+      <c r="K24" s="157">
         <f ca="1">IFERROR('Calculations 60Gy_8F'!L27/100,"??")</f>
-        <v>??</v>
+        <v>0.58700000000000008</v>
       </c>
       <c r="L24" s="80" t="str">
-        <f>'Calculations 60Gy_8F'!K33</f>
-        <v>??</v>
+        <f ca="1">'Calculations 60Gy_8F'!K33</f>
+        <v>Yes</v>
       </c>
       <c r="M24" s="140" t="s">
         <v>191</v>
       </c>
-      <c r="O24" s="303" t="str">
+      <c r="O24" s="302" t="str">
         <f>C30</f>
         <v>Mean Dose (Total lung)</v>
       </c>
-      <c r="P24" s="313" t="str">
+      <c r="P24" s="312">
         <f>G30</f>
-        <v>??</v>
+        <v>468</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -7988,40 +8026,40 @@
       <c r="C25" s="133" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="261" t="s">
+      <c r="D25" s="260" t="s">
         <v>180</v>
       </c>
       <c r="E25" s="90"/>
       <c r="F25" s="189"/>
-      <c r="G25" s="195" t="s">
-        <v>68</v>
-      </c>
-      <c r="H25" s="141" t="str">
+      <c r="G25" s="346">
+        <v>161.5</v>
+      </c>
+      <c r="H25" s="141">
         <f>IFERROR(G25/G9,"??")</f>
-        <v>??</v>
+        <v>4.3885869565217392</v>
       </c>
       <c r="I25" s="142" t="s">
         <v>37</v>
       </c>
       <c r="J25" s="90"/>
-      <c r="K25" s="158" t="str">
+      <c r="K25" s="158">
         <f ca="1">IFERROR('Calculations 60Gy_8F'!I27,"??")</f>
-        <v>??</v>
+        <v>4.2475000000000005</v>
       </c>
       <c r="L25" s="81" t="str">
-        <f>'Calculations 60Gy_8F'!K32</f>
-        <v>??</v>
+        <f ca="1">'Calculations 60Gy_8F'!K32</f>
+        <v>Minor Deviation</v>
       </c>
       <c r="M25" s="140" t="s">
         <v>192</v>
       </c>
-      <c r="O25" s="303" t="str">
+      <c r="O25" s="302" t="str">
         <f>C31</f>
         <v>V20 (Total Lung)</v>
       </c>
-      <c r="P25" s="313" t="str">
+      <c r="P25" s="312">
         <f>G31</f>
-        <v>??</v>
+        <v>5.5139066666666674E-2</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
@@ -8045,13 +8083,13 @@
       </c>
       <c r="L26" s="145"/>
       <c r="M26" s="87"/>
-      <c r="O26" s="303" t="str">
+      <c r="O26" s="302" t="str">
         <f>CONCATENATE(C33," ",F33)</f>
         <v>Aorta  (max point dose)</v>
       </c>
-      <c r="P26" s="313" t="str">
+      <c r="P26" s="312">
         <f>G33</f>
-        <v>??</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="27" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -8073,13 +8111,13 @@
       </c>
       <c r="L27" s="145"/>
       <c r="M27" s="87"/>
-      <c r="O27" s="303" t="str">
+      <c r="O27" s="302" t="str">
         <f>CONCATENATE(C33," ",F34)</f>
         <v>Aorta  V60Gy=</v>
       </c>
-      <c r="P27" s="313" t="str">
+      <c r="P27" s="312">
         <f t="shared" ref="P27:P37" si="0">G34</f>
-        <v>??</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
@@ -8099,13 +8137,13 @@
       <c r="K28" s="119"/>
       <c r="L28" s="11"/>
       <c r="M28" s="87"/>
-      <c r="O28" s="303" t="str">
+      <c r="O28" s="302" t="str">
         <f>CONCATENATE(C35," ",F35)</f>
         <v>Artery-Pulmonary (max point dose)</v>
       </c>
-      <c r="P28" s="313" t="str">
+      <c r="P28" s="312">
         <f t="shared" si="0"/>
-        <v>??</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
@@ -8116,8 +8154,8 @@
       <c r="D29" s="96"/>
       <c r="E29" s="96"/>
       <c r="F29" s="97"/>
-      <c r="G29" s="6" t="s">
-        <v>68</v>
+      <c r="G29" s="318">
+        <v>468</v>
       </c>
       <c r="H29" s="131"/>
       <c r="I29" s="122"/>
@@ -8127,13 +8165,13 @@
         <v>68</v>
       </c>
       <c r="M29" s="87"/>
-      <c r="O29" s="303" t="str">
+      <c r="O29" s="302" t="str">
         <f>CONCATENATE(C35," ",F36)</f>
         <v>Artery-Pulmonary V60Gy=</v>
       </c>
-      <c r="P29" s="313" t="str">
+      <c r="P29" s="312">
         <f t="shared" si="0"/>
-        <v>??</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
@@ -8144,8 +8182,8 @@
       <c r="D30" s="96"/>
       <c r="E30" s="96"/>
       <c r="F30" s="97"/>
-      <c r="G30" s="7" t="s">
-        <v>68</v>
+      <c r="G30" s="330">
+        <v>468</v>
       </c>
       <c r="H30" s="146"/>
       <c r="I30" s="147"/>
@@ -8155,13 +8193,13 @@
         <v>68</v>
       </c>
       <c r="M30" s="87"/>
-      <c r="O30" s="303" t="str">
+      <c r="O30" s="302" t="str">
         <f>CONCATENATE(C37," ",F37)</f>
         <v>Spinal Canal (max point dose)</v>
       </c>
-      <c r="P30" s="313" t="str">
+      <c r="P30" s="312">
         <f t="shared" si="0"/>
-        <v>??</v>
+        <v>906</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -8170,12 +8208,12 @@
         <v>27</v>
       </c>
       <c r="D31" s="90"/>
-      <c r="E31" s="322" t="s">
+      <c r="E31" s="340" t="s">
         <v>175</v>
       </c>
-      <c r="F31" s="323"/>
-      <c r="G31" s="196" t="s">
-        <v>68</v>
+      <c r="F31" s="341"/>
+      <c r="G31" s="196">
+        <v>5.5139066666666674E-2</v>
       </c>
       <c r="H31" s="186" t="s">
         <v>37</v>
@@ -8187,16 +8225,16 @@
       </c>
       <c r="L31" s="192" t="str">
         <f>'Calculations 60Gy_8F'!K34</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="M31" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="O31" s="303" t="str">
+      <c r="O31" s="302" t="str">
         <f>CONCATENATE(C38," ",F38)</f>
         <v>Ipsilat. Brach. Plex. (max point dose)</v>
       </c>
-      <c r="P31" s="313" t="str">
+      <c r="P31" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
@@ -8218,18 +8256,18 @@
       <c r="K32" s="128"/>
       <c r="L32" s="100"/>
       <c r="M32" s="87"/>
-      <c r="O32" s="303" t="str">
+      <c r="O32" s="302" t="str">
         <f>CONCATENATE(C38," ",F39)</f>
         <v>Ipsilat. Brach. Plex. V30Gy=</v>
       </c>
-      <c r="P32" s="313" t="str">
+      <c r="P32" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B33" s="94"/>
-      <c r="C33" s="205" t="s">
+      <c r="C33" s="204" t="s">
         <v>132</v>
       </c>
       <c r="D33" s="107" t="s">
@@ -8239,8 +8277,8 @@
       <c r="F33" s="178" t="s">
         <v>62</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>68</v>
+      <c r="G33" s="332">
+        <v>1812</v>
       </c>
       <c r="H33" s="115"/>
       <c r="I33" s="107"/>
@@ -8250,33 +8288,32 @@
       </c>
       <c r="L33" s="191" t="str">
         <f>IF(G33="??","??",IF(G33&lt;=6400,"Yes","No"))</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="M33" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="O33" s="303" t="str">
+      <c r="O33" s="302" t="str">
         <f>CONCATENATE(C40," ",F40)</f>
         <v>Heart (max point dose)</v>
       </c>
-      <c r="P33" s="313" t="str">
+      <c r="P33" s="312">
         <f t="shared" si="0"/>
-        <v>??</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B34" s="94"/>
-      <c r="C34" s="235"/>
-      <c r="D34" s="236" t="s">
+      <c r="C34" s="234"/>
+      <c r="D34" s="235" t="s">
         <v>152</v>
       </c>
       <c r="E34" s="147"/>
-      <c r="F34" s="262" t="s">
+      <c r="F34" s="261" t="s">
         <v>153</v>
       </c>
-      <c r="G34" s="4" t="str">
-        <f>IF(G33&lt;=6000,"OK","??")</f>
-        <v>??</v>
+      <c r="G34" s="334">
+        <v>0</v>
       </c>
       <c r="H34" s="115"/>
       <c r="I34" s="107"/>
@@ -8286,21 +8323,21 @@
       </c>
       <c r="L34" s="191" t="str">
         <f>IF(G34="??","??",IF(G34&lt;=10,"Yes",IF(G34="OK","Yes","No")))</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="M34" s="87"/>
-      <c r="O34" s="303" t="str">
+      <c r="O34" s="302" t="str">
         <f>CONCATENATE(C40," ",F41)</f>
         <v>Heart V60Gy=</v>
       </c>
-      <c r="P34" s="313" t="str">
+      <c r="P34" s="312">
         <f t="shared" si="0"/>
-        <v>??</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B35" s="94"/>
-      <c r="C35" s="205" t="s">
+      <c r="C35" s="204" t="s">
         <v>170</v>
       </c>
       <c r="D35" s="107"/>
@@ -8308,8 +8345,8 @@
       <c r="F35" s="178" t="s">
         <v>62</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>68</v>
+      <c r="G35" s="332">
+        <v>1134</v>
       </c>
       <c r="H35" s="115"/>
       <c r="I35" s="107"/>
@@ -8319,33 +8356,32 @@
       </c>
       <c r="L35" s="191" t="str">
         <f>IF(G35="??","??",IF(G35&lt;=6400,"Yes","No"))</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="M35" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="O35" s="303" t="str">
+      <c r="O35" s="302" t="str">
         <f>CONCATENATE(C42," ",F42)</f>
         <v>Esophagus (max point dose)</v>
       </c>
-      <c r="P35" s="313" t="str">
+      <c r="P35" s="312">
         <f t="shared" si="0"/>
-        <v>??</v>
+        <v>942</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B36" s="94"/>
-      <c r="C36" s="235"/>
-      <c r="D36" s="236" t="s">
+      <c r="C36" s="234"/>
+      <c r="D36" s="235" t="s">
         <v>152</v>
       </c>
       <c r="E36" s="147"/>
-      <c r="F36" s="262" t="s">
+      <c r="F36" s="261" t="s">
         <v>153</v>
       </c>
-      <c r="G36" s="4" t="str">
-        <f>IF(G35&lt;=6000,"OK","??")</f>
-        <v>??</v>
+      <c r="G36" s="334">
+        <v>0</v>
       </c>
       <c r="H36" s="115"/>
       <c r="I36" s="107"/>
@@ -8355,16 +8391,16 @@
       </c>
       <c r="L36" s="191" t="str">
         <f>IF(G36="??","??",IF(G36&lt;=10,"Yes",IF(G36="OK","Yes","No")))</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="M36" s="87"/>
-      <c r="O36" s="303" t="str">
+      <c r="O36" s="302" t="str">
         <f>CONCATENATE(C43," ",F43)</f>
         <v>Chestwall (rib) (max point dose)</v>
       </c>
-      <c r="P36" s="313" t="str">
+      <c r="P36" s="312">
         <f t="shared" si="0"/>
-        <v>??</v>
+        <v>7320</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
@@ -8377,8 +8413,8 @@
       <c r="F37" s="150" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="170" t="s">
-        <v>68</v>
+      <c r="G37" s="348">
+        <v>906</v>
       </c>
       <c r="H37" s="115"/>
       <c r="I37" s="107"/>
@@ -8388,23 +8424,23 @@
       </c>
       <c r="L37" s="191" t="str">
         <f>IF(G37="??","??",IF(G37&lt;=3200,"Yes","No"))</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="M37" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="O37" s="303" t="str">
+      <c r="O37" s="302" t="str">
         <f>CONCATENATE(C43," ",F44)</f>
         <v>Chestwall (rib) V50Gy=</v>
       </c>
-      <c r="P37" s="313" t="str">
+      <c r="P37" s="312">
         <f t="shared" si="0"/>
-        <v>??</v>
+        <v>8.6618669399999995</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B38" s="94"/>
-      <c r="C38" s="205" t="s">
+      <c r="C38" s="204" t="s">
         <v>189</v>
       </c>
       <c r="D38" s="107"/>
@@ -8428,23 +8464,23 @@
       <c r="M38" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="O38" s="303" t="str">
+      <c r="O38" s="302" t="str">
         <f>CONCATENATE(A44," ",F45)</f>
         <v>Trachea (max point dose)</v>
       </c>
-      <c r="P38" s="314">
+      <c r="P38" s="313">
         <f>A45</f>
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B39" s="94"/>
       <c r="C39" s="177"/>
-      <c r="D39" s="236" t="s">
+      <c r="D39" s="235" t="s">
         <v>206</v>
       </c>
       <c r="E39" s="147"/>
-      <c r="F39" s="263" t="s">
+      <c r="F39" s="262" t="s">
         <v>121</v>
       </c>
       <c r="G39" s="4" t="str">
@@ -8462,11 +8498,11 @@
         <v>??</v>
       </c>
       <c r="M39" s="140"/>
-      <c r="O39" s="303" t="str">
+      <c r="O39" s="302" t="str">
         <f>CONCATENATE(A44," ",F46)</f>
         <v>Trachea V60Gy =</v>
       </c>
-      <c r="P39" s="314">
+      <c r="P39" s="313">
         <f>A46</f>
         <v>0</v>
       </c>
@@ -8481,8 +8517,8 @@
       <c r="F40" s="179" t="s">
         <v>62</v>
       </c>
-      <c r="G40" s="170" t="s">
-        <v>68</v>
+      <c r="G40" s="348">
+        <v>1038</v>
       </c>
       <c r="H40" s="115"/>
       <c r="I40" s="107"/>
@@ -8492,33 +8528,32 @@
       </c>
       <c r="L40" s="191" t="str">
         <f>IF(G40="??","??",IF(G40&lt;=6400,"Yes","No"))</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="M40" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="O40" s="303" t="str">
+      <c r="O40" s="302" t="str">
         <f>CONCATENATE(B44," ",F45)</f>
         <v>Bronchus (max point dose)</v>
       </c>
-      <c r="P40" s="314">
+      <c r="P40" s="313">
         <f>B45</f>
-        <v>0</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="14.25" x14ac:dyDescent="0.25">
       <c r="B41" s="94"/>
-      <c r="C41" s="235"/>
-      <c r="D41" s="236" t="s">
+      <c r="C41" s="234"/>
+      <c r="D41" s="235" t="s">
         <v>152</v>
       </c>
       <c r="E41" s="147"/>
-      <c r="F41" s="262" t="s">
+      <c r="F41" s="261" t="s">
         <v>153</v>
       </c>
-      <c r="G41" s="4" t="str">
-        <f>IF(G40&lt;=6000,"OK","??")</f>
-        <v>??</v>
+      <c r="G41" s="334">
+        <v>0</v>
       </c>
       <c r="H41" s="115"/>
       <c r="I41" s="107"/>
@@ -8528,16 +8563,16 @@
       </c>
       <c r="L41" s="191" t="str">
         <f>IF(G41="??","??",IF(G41&lt;=10,"Yes",IF(G41="OK","Yes","No")))</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="M41" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="O41" s="303" t="str">
+      <c r="O41" s="302" t="str">
         <f>CONCATENATE(B44," ",F48)</f>
         <v>Bronchus V36Gy=</v>
       </c>
-      <c r="P41" s="314">
+      <c r="P41" s="313">
         <f>B46</f>
         <v>0</v>
       </c>
@@ -8552,8 +8587,8 @@
       <c r="F42" s="149" t="s">
         <v>62</v>
       </c>
-      <c r="G42" s="170" t="s">
-        <v>68</v>
+      <c r="G42" s="348">
+        <v>942</v>
       </c>
       <c r="H42" s="115"/>
       <c r="I42" s="107"/>
@@ -8563,18 +8598,18 @@
       </c>
       <c r="L42" s="191" t="str">
         <f>IF(G42="??","??",IF(G42&lt;=4000,"Yes","No"))</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="M42" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="O42" s="303" t="str">
+      <c r="O42" s="302" t="str">
         <f>CONCATENATE(C45," ",C46," ",F45)</f>
         <v>Proximal Trachea &amp; Bronch. Tree:  (max point dose)</v>
       </c>
-      <c r="P42" s="313" t="str">
+      <c r="P42" s="312">
         <f>G45</f>
-        <v>??</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -8587,8 +8622,8 @@
       <c r="F43" s="179" t="s">
         <v>62</v>
       </c>
-      <c r="G43" s="170" t="s">
-        <v>68</v>
+      <c r="G43" s="348">
+        <v>7320</v>
       </c>
       <c r="H43" s="115"/>
       <c r="I43" s="107"/>
@@ -8598,25 +8633,25 @@
       </c>
       <c r="L43" s="191" t="str">
         <f>IF(G43="??","??",IF(G43&lt;=6000,"Yes","No"))</f>
-        <v>??</v>
+        <v>No</v>
       </c>
       <c r="M43" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="O43" s="303" t="str">
+      <c r="O43" s="302" t="str">
         <f>CONCATENATE(C45," ",C46," ",F46)</f>
         <v>Proximal Trachea &amp; Bronch. Tree:  V60Gy =</v>
       </c>
-      <c r="P43" s="313" t="str">
+      <c r="P43" s="312" t="str">
         <f>G46</f>
         <v>??</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="294" t="s">
+      <c r="A44" s="293" t="s">
         <v>209</v>
       </c>
-      <c r="B44" s="295" t="s">
+      <c r="B44" s="294" t="s">
         <v>210</v>
       </c>
       <c r="C44" s="94"/>
@@ -8624,12 +8659,11 @@
         <v>168</v>
       </c>
       <c r="E44" s="147"/>
-      <c r="F44" s="262" t="s">
+      <c r="F44" s="261" t="s">
         <v>169</v>
       </c>
-      <c r="G44" s="4" t="str">
-        <f>IF(G43&lt;=5000,"OK","??")</f>
-        <v>??</v>
+      <c r="G44" s="334">
+        <v>8.6618669399999995</v>
       </c>
       <c r="H44" s="115"/>
       <c r="I44" s="107"/>
@@ -8639,40 +8673,40 @@
       </c>
       <c r="L44" s="191" t="str">
         <f>IF(G44="??","??",IF(G44&lt;=5,"Yes",IF(G44="OK","Yes","No")))</f>
-        <v>??</v>
+        <v>No</v>
       </c>
       <c r="M44" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="O44" s="303" t="str">
+      <c r="O44" s="302" t="str">
         <f>CONCATENATE(C47," ",C48," ",F47)</f>
         <v>Stomach and  Intestines (max point dose)</v>
       </c>
-      <c r="P44" s="313" t="str">
+      <c r="P44" s="312" t="str">
         <f>G47</f>
         <v>??</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A45" s="296">
-        <v>0</v>
-      </c>
-      <c r="B45" s="297">
-        <v>0</v>
+      <c r="A45" s="349">
+        <v>54</v>
+      </c>
+      <c r="B45" s="350">
+        <v>2316</v>
       </c>
       <c r="C45" s="151" t="s">
         <v>16</v>
       </c>
-      <c r="D45" s="291"/>
+      <c r="D45" s="290"/>
       <c r="E45" s="107"/>
       <c r="F45" s="149" t="s">
         <v>62</v>
       </c>
-      <c r="G45" s="194" t="str">
+      <c r="G45" s="194">
         <f>IF(MAX(A45:B45)&gt;0,MAX(A45:B45),"??")</f>
-        <v>??</v>
-      </c>
-      <c r="H45" s="292" t="s">
+        <v>2316</v>
+      </c>
+      <c r="H45" s="291" t="s">
         <v>37</v>
       </c>
       <c r="I45" s="122"/>
@@ -8682,25 +8716,25 @@
       </c>
       <c r="L45" s="191" t="str">
         <f>IF(G45="??","??",IF(G45&lt;=6400,"Yes","No"))</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="M45" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="O45" s="303" t="str">
+      <c r="O45" s="302" t="str">
         <f>CONCATENATE(C47," ",C48," ",F48)</f>
         <v>Stomach and  Intestines V36Gy=</v>
       </c>
-      <c r="P45" s="313" t="str">
+      <c r="P45" s="312" t="str">
         <f>G48</f>
         <v>??</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="298">
+      <c r="A46" s="351">
         <v>0</v>
       </c>
-      <c r="B46" s="299">
+      <c r="B46" s="352">
         <v>0</v>
       </c>
       <c r="C46" s="190" t="s">
@@ -8717,7 +8751,7 @@
         <f>IF(MAX(A46:B46)&gt;0,MAX(A46:B46),"??")</f>
         <v>??</v>
       </c>
-      <c r="H46" s="293" t="s">
+      <c r="H46" s="292" t="s">
         <v>37</v>
       </c>
       <c r="I46" s="96"/>
@@ -8732,11 +8766,11 @@
       <c r="M46" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="O46" s="303" t="str">
+      <c r="O46" s="302" t="str">
         <f>C49</f>
         <v>Dosimetrist:</v>
       </c>
-      <c r="P46" s="307" t="str">
+      <c r="P46" s="306" t="str">
         <f>C50</f>
         <v>??</v>
       </c>
@@ -8767,11 +8801,11 @@
       <c r="M47" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="O47" s="303" t="str">
+      <c r="O47" s="302" t="str">
         <f>G49</f>
         <v>Physicist:</v>
       </c>
-      <c r="P47" s="307" t="str">
+      <c r="P47" s="306" t="str">
         <f>G50</f>
         <v>??</v>
       </c>
@@ -8781,13 +8815,13 @@
       <c r="C48" s="89" t="s">
         <v>138</v>
       </c>
-      <c r="D48" s="228" t="s">
+      <c r="D48" s="227" t="s">
         <v>207</v>
       </c>
       <c r="E48" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="F48" s="264" t="s">
+      <c r="F48" s="263" t="s">
         <v>131</v>
       </c>
       <c r="G48" s="193" t="str">
@@ -8807,11 +8841,11 @@
       <c r="M48" s="140" t="s">
         <v>167</v>
       </c>
-      <c r="O48" s="303" t="str">
+      <c r="O48" s="302" t="str">
         <f>K49</f>
         <v>Radiation Oncologist:</v>
       </c>
-      <c r="P48" s="307" t="str">
+      <c r="P48" s="306" t="str">
         <f>K50</f>
         <v>??</v>
       </c>
@@ -8837,11 +8871,11 @@
       </c>
       <c r="L49" s="100"/>
       <c r="M49" s="87"/>
-      <c r="O49" s="303" t="str">
+      <c r="O49" s="302" t="str">
         <f>B51</f>
         <v>NOTES:</v>
       </c>
-      <c r="P49" s="307">
+      <c r="P49" s="306">
         <f>C51</f>
         <v>0</v>
       </c>
@@ -8865,7 +8899,7 @@
       </c>
       <c r="L50" s="100"/>
       <c r="M50" s="87"/>
-      <c r="P50" s="315"/>
+      <c r="P50" s="314"/>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B51" s="101" t="s">
@@ -8882,24 +8916,24 @@
       <c r="K51" s="22"/>
       <c r="L51" s="17"/>
       <c r="M51" s="87"/>
-      <c r="P51" s="315"/>
+      <c r="P51" s="314"/>
     </row>
     <row r="52" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="89"/>
-      <c r="C52" s="265"/>
-      <c r="D52" s="265"/>
-      <c r="E52" s="265"/>
-      <c r="F52" s="266"/>
-      <c r="G52" s="266"/>
-      <c r="H52" s="267" t="s">
+      <c r="C52" s="264"/>
+      <c r="D52" s="264"/>
+      <c r="E52" s="264"/>
+      <c r="F52" s="265"/>
+      <c r="G52" s="265"/>
+      <c r="H52" s="266" t="s">
         <v>37</v>
       </c>
-      <c r="I52" s="265"/>
-      <c r="J52" s="265"/>
-      <c r="K52" s="266"/>
-      <c r="L52" s="268"/>
+      <c r="I52" s="264"/>
+      <c r="J52" s="264"/>
+      <c r="K52" s="265"/>
+      <c r="L52" s="267"/>
       <c r="M52" s="87"/>
-      <c r="P52" s="315"/>
+      <c r="P52" s="314"/>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B53" s="153" t="s">
@@ -8916,7 +8950,7 @@
       <c r="K53" s="154"/>
       <c r="L53" s="154"/>
       <c r="M53" s="87"/>
-      <c r="P53" s="315"/>
+      <c r="P53" s="314"/>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B54" s="88"/>
@@ -8931,7 +8965,7 @@
       <c r="K54" s="154"/>
       <c r="L54" s="154"/>
       <c r="M54" s="87"/>
-      <c r="P54" s="315"/>
+      <c r="P54" s="314"/>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B55" s="88"/>
@@ -8946,7 +8980,7 @@
       <c r="K55" s="154"/>
       <c r="L55" s="154"/>
       <c r="M55" s="87"/>
-      <c r="P55" s="315"/>
+      <c r="P55" s="314"/>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B56" s="88"/>
@@ -8961,20 +8995,20 @@
       <c r="K56" s="154"/>
       <c r="L56" s="154"/>
       <c r="M56" s="87"/>
-      <c r="P56" s="315"/>
+      <c r="P56" s="314"/>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.2">
       <c r="M57" s="87"/>
-      <c r="P57" s="315"/>
+      <c r="P57" s="314"/>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="P58" s="315"/>
+      <c r="P58" s="314"/>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="P59" s="315"/>
+      <c r="P59" s="314"/>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="P60" s="315"/>
+      <c r="P60" s="314"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
@@ -9035,7 +9069,7 @@
   </sheetPr>
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -9054,28 +9088,28 @@
     <col min="11" max="11" width="13.85546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="15.5703125" style="1" customWidth="1"/>
     <col min="13" max="13" width="14" style="2" customWidth="1"/>
-    <col min="15" max="15" width="52.42578125" style="301" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" style="304" customWidth="1"/>
+    <col min="15" max="15" width="52.42578125" style="300" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" style="303" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="206" t="s">
+      <c r="B1" s="205" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="207"/>
-      <c r="D1" s="206"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="208"/>
-      <c r="G1" s="208"/>
-      <c r="H1" s="209" t="s">
+      <c r="C1" s="206"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="206"/>
+      <c r="F1" s="207"/>
+      <c r="G1" s="207"/>
+      <c r="H1" s="208" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="206"/>
-      <c r="J1" s="206"/>
-      <c r="K1" s="210"/>
-      <c r="L1" s="210"/>
+      <c r="I1" s="205"/>
+      <c r="J1" s="205"/>
+      <c r="K1" s="209"/>
+      <c r="L1" s="209"/>
       <c r="M1" s="87"/>
-      <c r="O1" s="300"/>
+      <c r="O1" s="299"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="82"/>
@@ -9092,7 +9126,7 @@
       <c r="K2" s="84"/>
       <c r="L2" s="86"/>
       <c r="M2" s="87"/>
-      <c r="O2" s="300"/>
+      <c r="O2" s="299"/>
     </row>
     <row r="3" spans="2:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="89"/>
@@ -9109,14 +9143,14 @@
       <c r="K3" s="91"/>
       <c r="L3" s="93"/>
       <c r="M3" s="87"/>
-      <c r="O3" s="300"/>
+      <c r="O3" s="299"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="94"/>
       <c r="C4" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="326" t="s">
+      <c r="D4" s="319" t="s">
         <v>213</v>
       </c>
       <c r="E4" s="96"/>
@@ -9124,7 +9158,7 @@
         <v>174</v>
       </c>
       <c r="G4" s="97"/>
-      <c r="H4" s="331">
+      <c r="H4" s="324">
         <v>5400</v>
       </c>
       <c r="I4" s="96"/>
@@ -9136,11 +9170,11 @@
         <v>75</v>
       </c>
       <c r="M4" s="87"/>
-      <c r="O4" s="303" t="str">
+      <c r="O4" s="302" t="str">
         <f>C4</f>
         <v>Patient:</v>
       </c>
-      <c r="P4" s="305" t="str">
+      <c r="P4" s="304" t="str">
         <f>D4</f>
         <v>PT1</v>
       </c>
@@ -9166,15 +9200,15 @@
       <c r="K5" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="327" t="s">
+      <c r="L5" s="320" t="s">
         <v>214</v>
       </c>
       <c r="M5" s="87"/>
-      <c r="O5" s="303" t="str">
+      <c r="O5" s="302" t="str">
         <f>C5</f>
         <v>CR#:</v>
       </c>
-      <c r="P5" s="306">
+      <c r="P5" s="305">
         <f>D5</f>
         <v>1</v>
       </c>
@@ -9194,11 +9228,11 @@
       <c r="K6" s="84"/>
       <c r="L6" s="86"/>
       <c r="M6" s="87"/>
-      <c r="O6" s="303" t="str">
+      <c r="O6" s="302" t="str">
         <f>K4</f>
         <v>Site:</v>
       </c>
-      <c r="P6" s="307" t="str">
+      <c r="P6" s="306" t="str">
         <f>L4</f>
         <v>LUNG</v>
       </c>
@@ -9211,7 +9245,7 @@
       <c r="D7" s="96"/>
       <c r="E7" s="96"/>
       <c r="F7" s="97"/>
-      <c r="G7" s="328">
+      <c r="G7" s="321">
         <v>1.3</v>
       </c>
       <c r="H7" s="97"/>
@@ -9220,11 +9254,11 @@
       <c r="K7" s="97"/>
       <c r="L7" s="100"/>
       <c r="M7" s="87"/>
-      <c r="O7" s="303" t="str">
+      <c r="O7" s="302" t="str">
         <f>K5</f>
         <v>Plan Name:</v>
       </c>
-      <c r="P7" s="306" t="str">
+      <c r="P7" s="305" t="str">
         <f>L5</f>
         <v>LUNR</v>
       </c>
@@ -9237,7 +9271,7 @@
       <c r="D8" s="96"/>
       <c r="E8" s="96"/>
       <c r="F8" s="97"/>
-      <c r="G8" s="329">
+      <c r="G8" s="322">
         <v>1.3</v>
       </c>
       <c r="H8" s="97"/>
@@ -9246,11 +9280,11 @@
       <c r="K8" s="97"/>
       <c r="L8" s="100"/>
       <c r="M8" s="87"/>
-      <c r="O8" s="303" t="str">
+      <c r="O8" s="302" t="str">
         <f>F4</f>
         <v>Prescription Dose (cGy):</v>
       </c>
-      <c r="P8" s="305">
+      <c r="P8" s="304">
         <f>H4</f>
         <v>5400</v>
       </c>
@@ -9263,7 +9297,7 @@
       <c r="D9" s="96"/>
       <c r="E9" s="96"/>
       <c r="F9" s="97"/>
-      <c r="G9" s="328">
+      <c r="G9" s="321">
         <v>7.3</v>
       </c>
       <c r="H9" s="97"/>
@@ -9272,11 +9306,11 @@
       <c r="K9" s="97"/>
       <c r="L9" s="100"/>
       <c r="M9" s="87"/>
-      <c r="O9" s="303" t="str">
+      <c r="O9" s="302" t="str">
         <f>F5</f>
         <v>Fractions:</v>
       </c>
-      <c r="P9" s="308">
+      <c r="P9" s="307">
         <f>H5</f>
         <v>3</v>
       </c>
@@ -9289,7 +9323,7 @@
       <c r="D10" s="90"/>
       <c r="E10" s="90"/>
       <c r="F10" s="91"/>
-      <c r="G10" s="330">
+      <c r="G10" s="323">
         <v>4689.5</v>
       </c>
       <c r="H10" s="91"/>
@@ -9298,11 +9332,11 @@
       <c r="K10" s="91"/>
       <c r="L10" s="93"/>
       <c r="M10" s="87"/>
-      <c r="O10" s="303" t="str">
+      <c r="O10" s="302" t="str">
         <f>C7</f>
         <v>GTV Volume (cc)</v>
       </c>
-      <c r="P10" s="309">
+      <c r="P10" s="308">
         <f>G7</f>
         <v>1.3</v>
       </c>
@@ -9313,28 +9347,28 @@
       </c>
       <c r="C11" s="83"/>
       <c r="D11" s="83"/>
-      <c r="E11" s="211" t="s">
+      <c r="E11" s="210" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="212"/>
-      <c r="G11" s="212"/>
-      <c r="H11" s="212"/>
+      <c r="F11" s="211"/>
+      <c r="G11" s="211"/>
+      <c r="H11" s="211"/>
       <c r="I11" s="117" t="s">
         <v>37</v>
       </c>
       <c r="J11" s="83"/>
-      <c r="K11" s="214" t="s">
+      <c r="K11" s="213" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="215" t="s">
+      <c r="L11" s="214" t="s">
         <v>37</v>
       </c>
       <c r="M11" s="87"/>
-      <c r="O11" s="303" t="str">
+      <c r="O11" s="302" t="str">
         <f>C8</f>
         <v>ITV Volume (cc):</v>
       </c>
-      <c r="P11" s="309">
+      <c r="P11" s="308">
         <f>G8</f>
         <v>1.3</v>
       </c>
@@ -9364,11 +9398,11 @@
       <c r="M12" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="O12" s="303" t="str">
+      <c r="O12" s="302" t="str">
         <f>C9</f>
         <v>PTV Volume (cc)</v>
       </c>
-      <c r="P12" s="310">
+      <c r="P12" s="309">
         <f>G9</f>
         <v>7.3</v>
       </c>
@@ -9390,11 +9424,11 @@
       </c>
       <c r="L13" s="100"/>
       <c r="M13" s="87"/>
-      <c r="O13" s="303" t="str">
+      <c r="O13" s="302" t="str">
         <f>C10</f>
         <v>Total Lung Volume (cc)</v>
       </c>
-      <c r="P13" s="309">
+      <c r="P13" s="308">
         <f>G10</f>
         <v>4689.5</v>
       </c>
@@ -9407,14 +9441,14 @@
       <c r="D14" s="107"/>
       <c r="E14" s="107"/>
       <c r="F14" s="115"/>
-      <c r="G14" s="269" t="str">
+      <c r="G14" s="268" t="str">
         <f>IFERROR(H14*$H$4,"??")</f>
         <v>??</v>
       </c>
       <c r="H14" s="168" t="s">
         <v>68</v>
       </c>
-      <c r="I14" s="220" t="b">
+      <c r="I14" s="219" t="b">
         <f>AND((H14&gt;59.99%),(H14&lt;90.01%))</f>
         <v>0</v>
       </c>
@@ -9429,11 +9463,11 @@
       <c r="M14" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="O14" s="303" t="str">
+      <c r="O14" s="302" t="str">
         <f>C14</f>
         <v>Plan Normalization Value (%)</v>
       </c>
-      <c r="P14" s="311" t="str">
+      <c r="P14" s="310" t="str">
         <f>H14</f>
         <v>??</v>
       </c>
@@ -9449,11 +9483,11 @@
       <c r="G15" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="219" t="str">
+      <c r="H15" s="218" t="str">
         <f>IFERROR(G15/$H$4,"??")</f>
         <v>??</v>
       </c>
-      <c r="I15" s="220" t="b">
+      <c r="I15" s="219" t="b">
         <f>AND((H15&gt;111%),(H15&lt;166.8%))</f>
         <v>0</v>
       </c>
@@ -9470,11 +9504,11 @@
       <c r="M15" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="O15" s="303" t="str">
+      <c r="O15" s="302" t="str">
         <f>C15</f>
         <v>Dose @COM-PTV (cGy)</v>
       </c>
-      <c r="P15" s="311" t="str">
+      <c r="P15" s="310" t="str">
         <f>G15</f>
         <v>??</v>
       </c>
@@ -9487,18 +9521,18 @@
       <c r="D16" s="83"/>
       <c r="E16" s="83"/>
       <c r="F16" s="118"/>
-      <c r="G16" s="221"/>
+      <c r="G16" s="220"/>
       <c r="H16" s="84"/>
-      <c r="I16" s="222"/>
+      <c r="I16" s="221"/>
       <c r="J16" s="83"/>
       <c r="K16" s="119"/>
       <c r="L16" s="11"/>
       <c r="M16" s="87"/>
-      <c r="O16" s="303" t="str">
+      <c r="O16" s="302" t="str">
         <f>C17</f>
         <v>PTV- Minimum Dose</v>
       </c>
-      <c r="P16" s="309">
+      <c r="P16" s="308">
         <f>G17</f>
         <v>0.90918518518518521</v>
       </c>
@@ -9511,14 +9545,14 @@
       <c r="D17" s="107"/>
       <c r="E17" s="107"/>
       <c r="F17" s="115"/>
-      <c r="G17" s="332">
+      <c r="G17" s="325">
         <v>0.90918518518518521</v>
       </c>
-      <c r="H17" s="223">
+      <c r="H17" s="222">
         <f>IFERROR(G17/$H$4,"??")</f>
         <v>1.6836762688614542E-4</v>
       </c>
-      <c r="I17" s="220" t="b">
+      <c r="I17" s="219" t="b">
         <f>AND((H17&gt;59.99%),(H17&lt;90.01%))</f>
         <v>0</v>
       </c>
@@ -9531,11 +9565,11 @@
         <v>No</v>
       </c>
       <c r="M17" s="87"/>
-      <c r="O17" s="303" t="str">
+      <c r="O17" s="302" t="str">
         <f>C18</f>
         <v>PTV - V100(%)</v>
       </c>
-      <c r="P17" s="312">
+      <c r="P17" s="311">
         <f>H18</f>
         <v>0.95586712328767121</v>
       </c>
@@ -9548,11 +9582,11 @@
       <c r="D18" s="96"/>
       <c r="E18" s="96"/>
       <c r="F18" s="97"/>
-      <c r="G18" s="270">
+      <c r="G18" s="269">
         <f>H4</f>
         <v>5400</v>
       </c>
-      <c r="H18" s="333">
+      <c r="H18" s="326">
         <v>0.95586712328767121</v>
       </c>
       <c r="I18" s="122"/>
@@ -9567,11 +9601,11 @@
       <c r="M18" s="88" t="s">
         <v>154</v>
       </c>
-      <c r="O18" s="303" t="str">
+      <c r="O18" s="302" t="str">
         <f>C19</f>
         <v>PTV - V90 (%)</v>
       </c>
-      <c r="P18" s="312">
+      <c r="P18" s="311">
         <f>H19</f>
         <v>1.006176712328767</v>
       </c>
@@ -9584,11 +9618,11 @@
       <c r="D19" s="90"/>
       <c r="E19" s="90"/>
       <c r="F19" s="91"/>
-      <c r="G19" s="271">
+      <c r="G19" s="270">
         <f>0.9*H4</f>
         <v>4860</v>
       </c>
-      <c r="H19" s="334">
+      <c r="H19" s="327">
         <v>1.006176712328767</v>
       </c>
       <c r="I19" s="126"/>
@@ -9603,11 +9637,11 @@
       <c r="M19" s="88" t="s">
         <v>155</v>
       </c>
-      <c r="O19" s="303" t="str">
+      <c r="O19" s="302" t="str">
         <f>CONCATENATE(C21," ",D21)</f>
         <v>Location V105% - PTV (cc) =</v>
       </c>
-      <c r="P19" s="312">
+      <c r="P19" s="311">
         <f>G21</f>
         <v>0</v>
       </c>
@@ -9621,17 +9655,17 @@
       <c r="E20" s="96"/>
       <c r="F20" s="97"/>
       <c r="G20" s="128"/>
-      <c r="H20" s="272"/>
+      <c r="H20" s="271"/>
       <c r="I20" s="96"/>
       <c r="J20" s="96"/>
       <c r="K20" s="129"/>
       <c r="L20" s="14"/>
       <c r="M20" s="87"/>
-      <c r="O20" s="303" t="str">
+      <c r="O20" s="302" t="str">
         <f>CONCATENATE(C22," ",D22)</f>
         <v>Volume V100% (cc) =</v>
       </c>
-      <c r="P20" s="312">
+      <c r="P20" s="311">
         <f>G22</f>
         <v>7.9</v>
       </c>
@@ -9648,7 +9682,7 @@
       </c>
       <c r="E21" s="122"/>
       <c r="F21" s="131"/>
-      <c r="G21" s="335">
+      <c r="G21" s="328">
         <v>0</v>
       </c>
       <c r="H21" s="172">
@@ -9667,11 +9701,11 @@
       <c r="M21" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="O21" s="303" t="str">
+      <c r="O21" s="302" t="str">
         <f>CONCATENATE(C24," ",D24)</f>
         <v>Location  D³2cm (%) =</v>
       </c>
-      <c r="P21" s="313">
+      <c r="P21" s="312">
         <f>G24</f>
         <v>48.61296296296296</v>
       </c>
@@ -9688,7 +9722,7 @@
       </c>
       <c r="E22" s="90"/>
       <c r="F22" s="91"/>
-      <c r="G22" s="336">
+      <c r="G22" s="329">
         <v>7.9</v>
       </c>
       <c r="H22" s="173">
@@ -9709,11 +9743,11 @@
       <c r="M22" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="O22" s="303" t="str">
+      <c r="O22" s="302" t="str">
         <f>C25</f>
         <v>Volume(R50)</v>
       </c>
-      <c r="P22" s="313">
+      <c r="P22" s="312">
         <f>G25</f>
         <v>38.9</v>
       </c>
@@ -9727,17 +9761,17 @@
       <c r="E23" s="83"/>
       <c r="F23" s="84"/>
       <c r="G23" s="119"/>
-      <c r="H23" s="273"/>
+      <c r="H23" s="272"/>
       <c r="I23" s="83"/>
       <c r="J23" s="83"/>
       <c r="K23" s="119"/>
       <c r="L23" s="11"/>
       <c r="M23" s="87"/>
-      <c r="O23" s="303" t="str">
+      <c r="O23" s="302" t="str">
         <f>C29</f>
         <v>Mean Dose (contralateral lung)</v>
       </c>
-      <c r="P23" s="313">
+      <c r="P23" s="312">
         <f>G29</f>
         <v>173.7</v>
       </c>
@@ -9754,10 +9788,10 @@
       </c>
       <c r="E24" s="122"/>
       <c r="F24" s="131"/>
-      <c r="G24" s="319">
+      <c r="G24" s="318">
         <v>48.61296296296296</v>
       </c>
-      <c r="H24" s="318">
+      <c r="H24" s="317">
         <f>IFERROR(G24/H4,"??")</f>
         <v>9.0024005486968438E-3</v>
       </c>
@@ -9774,11 +9808,11 @@
       <c r="M24" s="140" t="s">
         <v>55</v>
       </c>
-      <c r="O24" s="303" t="str">
+      <c r="O24" s="302" t="str">
         <f>C30</f>
         <v>Mean Dose (Total lung)</v>
       </c>
-      <c r="P24" s="313">
+      <c r="P24" s="312">
         <f>G30</f>
         <v>173.7</v>
       </c>
@@ -9795,7 +9829,7 @@
       <c r="F25" s="183" t="s">
         <v>163</v>
       </c>
-      <c r="G25" s="336">
+      <c r="G25" s="329">
         <v>38.9</v>
       </c>
       <c r="H25" s="141">
@@ -9817,11 +9851,11 @@
       <c r="M25" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="O25" s="303" t="str">
+      <c r="O25" s="302" t="str">
         <f>C31</f>
         <v>V20 (Total Lung) in %</v>
       </c>
-      <c r="P25" s="313">
+      <c r="P25" s="312">
         <f>G31</f>
         <v>1.4668301524682802E-2</v>
       </c>
@@ -9847,11 +9881,11 @@
       </c>
       <c r="L26" s="145"/>
       <c r="M26" s="87"/>
-      <c r="O26" s="303" t="str">
+      <c r="O26" s="302" t="str">
         <f>CONCATENATE(C32," ",F32)</f>
         <v>Lung-Basic Function V11.6Gy=</v>
       </c>
-      <c r="P26" s="313">
+      <c r="P26" s="312">
         <f>G32</f>
         <v>161.52199999999999</v>
       </c>
@@ -9867,19 +9901,19 @@
       <c r="G27" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="H27" s="272"/>
+      <c r="H27" s="271"/>
       <c r="I27" s="143"/>
       <c r="J27" s="143"/>
-      <c r="K27" s="274" t="s">
+      <c r="K27" s="273" t="s">
         <v>61</v>
       </c>
       <c r="L27" s="145"/>
       <c r="M27" s="87"/>
-      <c r="O27" s="303" t="str">
+      <c r="O27" s="302" t="str">
         <f>CONCATENATE(C33," ",F33)</f>
         <v>Lung-Pneumonitis V12.4Gy=</v>
       </c>
-      <c r="P27" s="313">
+      <c r="P27" s="312">
         <f>G33</f>
         <v>146.46199999999999</v>
       </c>
@@ -9895,17 +9929,17 @@
       <c r="E28" s="83"/>
       <c r="F28" s="84"/>
       <c r="G28" s="119"/>
-      <c r="H28" s="273"/>
+      <c r="H28" s="272"/>
       <c r="I28" s="83"/>
       <c r="J28" s="83"/>
       <c r="K28" s="119"/>
       <c r="L28" s="11"/>
       <c r="M28" s="87"/>
-      <c r="O28" s="303" t="str">
+      <c r="O28" s="302" t="str">
         <f>CONCATENATE(C35," ",F35)</f>
         <v>Aorta  (max point dose)</v>
       </c>
-      <c r="P28" s="313">
+      <c r="P28" s="312">
         <f>G35</f>
         <v>675.6</v>
       </c>
@@ -9918,20 +9952,20 @@
       <c r="D29" s="96"/>
       <c r="E29" s="96"/>
       <c r="F29" s="97"/>
-      <c r="G29" s="319">
+      <c r="G29" s="318">
         <v>173.7</v>
       </c>
       <c r="H29" s="181"/>
       <c r="I29" s="122"/>
       <c r="J29" s="122"/>
       <c r="K29" s="16"/>
-      <c r="L29" s="275"/>
+      <c r="L29" s="274"/>
       <c r="M29" s="87"/>
-      <c r="O29" s="303" t="str">
+      <c r="O29" s="302" t="str">
         <f>CONCATENATE(C36," ",F35)</f>
         <v>Artery-Pulmnory (max point dose)</v>
       </c>
-      <c r="P29" s="313">
+      <c r="P29" s="312">
         <f t="shared" ref="P29:P38" si="0">G36</f>
         <v>606.79999999999995</v>
       </c>
@@ -9944,20 +9978,20 @@
       <c r="D30" s="96"/>
       <c r="E30" s="96"/>
       <c r="F30" s="97"/>
-      <c r="G30" s="337">
+      <c r="G30" s="330">
         <v>173.7</v>
       </c>
-      <c r="H30" s="276"/>
+      <c r="H30" s="275"/>
       <c r="I30" s="147"/>
       <c r="J30" s="147"/>
       <c r="K30" s="148"/>
-      <c r="L30" s="277"/>
+      <c r="L30" s="276"/>
       <c r="M30" s="87"/>
-      <c r="O30" s="303" t="str">
+      <c r="O30" s="302" t="str">
         <f>CONCATENATE(C37," ",F37)</f>
         <v>Spinal Canal (max point dose)</v>
       </c>
-      <c r="P30" s="313">
+      <c r="P30" s="312">
         <f t="shared" si="0"/>
         <v>681.8</v>
       </c>
@@ -9980,7 +10014,7 @@
       </c>
       <c r="I31" s="122"/>
       <c r="J31" s="122"/>
-      <c r="K31" s="278">
+      <c r="K31" s="277">
         <f ca="1">IFERROR('Calculations 54Gy 3F'!O27,"??")</f>
         <v>10</v>
       </c>
@@ -9991,11 +10025,11 @@
       <c r="M31" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="O31" s="303" t="str">
+      <c r="O31" s="302" t="str">
         <f>CONCATENATE(C38," ",F37)</f>
         <v>Spinal Canal-PRV 5mm (max point dose)</v>
       </c>
-      <c r="P31" s="313">
+      <c r="P31" s="312">
         <f t="shared" si="0"/>
         <v>722</v>
       </c>
@@ -10007,18 +10041,18 @@
       </c>
       <c r="D32" s="96"/>
       <c r="E32" s="96"/>
-      <c r="F32" s="272" t="s">
+      <c r="F32" s="271" t="s">
         <v>133</v>
       </c>
-      <c r="G32" s="319">
+      <c r="G32" s="318">
         <v>161.52199999999999</v>
       </c>
-      <c r="H32" s="231" t="s">
+      <c r="H32" s="230" t="s">
         <v>151</v>
       </c>
       <c r="I32" s="122"/>
       <c r="J32" s="122"/>
-      <c r="K32" s="278">
+      <c r="K32" s="277">
         <v>1500</v>
       </c>
       <c r="L32" s="191" t="str">
@@ -10028,11 +10062,11 @@
       <c r="M32" s="140" t="s">
         <v>73</v>
       </c>
-      <c r="O32" s="303" t="str">
+      <c r="O32" s="302" t="str">
         <f>CONCATENATE(C39," ",F39)</f>
         <v>Ipsilat Brach.Plex (max point dose)</v>
       </c>
-      <c r="P32" s="313" t="str">
+      <c r="P32" s="312" t="str">
         <f t="shared" si="0"/>
         <v>??</v>
       </c>
@@ -10047,10 +10081,10 @@
       <c r="F33" s="97" t="s">
         <v>134</v>
       </c>
-      <c r="G33" s="338">
+      <c r="G33" s="331">
         <v>146.46199999999999</v>
       </c>
-      <c r="H33" s="231" t="s">
+      <c r="H33" s="230" t="s">
         <v>149</v>
       </c>
       <c r="I33" s="96"/>
@@ -10065,11 +10099,11 @@
       <c r="M33" s="140" t="s">
         <v>74</v>
       </c>
-      <c r="O33" s="303" t="str">
+      <c r="O33" s="302" t="str">
         <f>CONCATENATE(C40," ",F40)</f>
         <v>Skin V30Gy=</v>
       </c>
-      <c r="P33" s="313">
+      <c r="P33" s="312">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -10091,18 +10125,18 @@
       <c r="K34" s="119"/>
       <c r="L34" s="86"/>
       <c r="M34" s="87"/>
-      <c r="O34" s="303" t="str">
+      <c r="O34" s="302" t="str">
         <f>CONCATENATE(C41," ",F41)</f>
         <v>Heart (max point dose)</v>
       </c>
-      <c r="P34" s="313">
+      <c r="P34" s="312">
         <f t="shared" si="0"/>
         <v>851.5</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B35" s="94"/>
-      <c r="C35" s="205" t="s">
+      <c r="C35" s="204" t="s">
         <v>132</v>
       </c>
       <c r="D35" s="107" t="s">
@@ -10112,7 +10146,7 @@
       <c r="F35" s="149" t="s">
         <v>62</v>
       </c>
-      <c r="G35" s="339">
+      <c r="G35" s="332">
         <v>675.6</v>
       </c>
       <c r="H35" s="115"/>
@@ -10126,11 +10160,11 @@
         <v>Yes</v>
       </c>
       <c r="M35" s="87"/>
-      <c r="O35" s="303" t="str">
+      <c r="O35" s="302" t="str">
         <f>CONCATENATE(C42," ",F42)</f>
         <v>Esophagus (max point dose)</v>
       </c>
-      <c r="P35" s="313">
+      <c r="P35" s="312">
         <f t="shared" si="0"/>
         <v>691.2</v>
       </c>
@@ -10143,7 +10177,7 @@
       <c r="D36" s="96"/>
       <c r="E36" s="96"/>
       <c r="F36" s="97"/>
-      <c r="G36" s="339">
+      <c r="G36" s="332">
         <v>606.79999999999995</v>
       </c>
       <c r="H36" s="115"/>
@@ -10157,11 +10191,11 @@
         <v>Yes</v>
       </c>
       <c r="M36" s="87"/>
-      <c r="O36" s="303" t="str">
+      <c r="O36" s="302" t="str">
         <f>CONCATENATE(C43," ",F43)</f>
         <v>*Chestwall (rib) (max point dose)</v>
       </c>
-      <c r="P36" s="313">
+      <c r="P36" s="312">
         <f t="shared" si="0"/>
         <v>2605.1</v>
       </c>
@@ -10179,7 +10213,7 @@
       <c r="G37" s="15">
         <v>681.8</v>
       </c>
-      <c r="H37" s="279" t="s">
+      <c r="H37" s="278" t="s">
         <v>37</v>
       </c>
       <c r="I37" s="107"/>
@@ -10194,24 +10228,24 @@
       <c r="M37" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="O37" s="303" t="str">
+      <c r="O37" s="302" t="str">
         <f>CONCATENATE(C43," ",F44)</f>
         <v>*Chestwall (rib) V28.2Gy=</v>
       </c>
-      <c r="P37" s="313">
+      <c r="P37" s="312">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B38" s="94"/>
-      <c r="C38" s="243" t="s">
+      <c r="C38" s="242" t="s">
         <v>35</v>
       </c>
       <c r="D38" s="122"/>
       <c r="E38" s="122"/>
       <c r="F38" s="131"/>
-      <c r="G38" s="319">
+      <c r="G38" s="318">
         <v>722</v>
       </c>
       <c r="H38" s="131"/>
@@ -10225,11 +10259,11 @@
         <v>Yes</v>
       </c>
       <c r="M38" s="87"/>
-      <c r="O38" s="303" t="str">
+      <c r="O38" s="302" t="str">
         <f>CONCATENATE(C43," ",F45)</f>
         <v>*Chestwall (rib) V30Gy=</v>
       </c>
-      <c r="P38" s="313">
+      <c r="P38" s="312">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -10241,7 +10275,7 @@
       </c>
       <c r="D39" s="107"/>
       <c r="E39" s="107"/>
-      <c r="F39" s="280" t="s">
+      <c r="F39" s="279" t="s">
         <v>62</v>
       </c>
       <c r="G39" s="5" t="s">
@@ -10260,50 +10294,50 @@
       <c r="M39" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="O39" s="303" t="str">
+      <c r="O39" s="302" t="str">
         <f>A46</f>
         <v>Trachea</v>
       </c>
-      <c r="P39" s="314">
+      <c r="P39" s="313">
         <f>A47</f>
         <v>10.4</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B40" s="94"/>
-      <c r="C40" s="281" t="s">
+      <c r="C40" s="280" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="282" t="s">
+      <c r="D40" s="281" t="s">
         <v>157</v>
       </c>
-      <c r="E40" s="283"/>
-      <c r="F40" s="284" t="s">
+      <c r="E40" s="282"/>
+      <c r="F40" s="283" t="s">
         <v>158</v>
       </c>
-      <c r="G40" s="340">
+      <c r="G40" s="333">
         <v>0</v>
       </c>
-      <c r="H40" s="285" t="s">
+      <c r="H40" s="284" t="s">
         <v>37</v>
       </c>
-      <c r="I40" s="286"/>
-      <c r="J40" s="286"/>
-      <c r="K40" s="287">
+      <c r="I40" s="285"/>
+      <c r="J40" s="285"/>
+      <c r="K40" s="286">
         <v>10</v>
       </c>
-      <c r="L40" s="288" t="str">
+      <c r="L40" s="287" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
       <c r="M40" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="O40" s="303" t="str">
+      <c r="O40" s="302" t="str">
         <f>B46</f>
         <v>Bronchus</v>
       </c>
-      <c r="P40" s="314">
+      <c r="P40" s="313">
         <f>B47</f>
         <v>1194</v>
       </c>
@@ -10321,7 +10355,7 @@
       <c r="G41" s="15">
         <v>851.5</v>
       </c>
-      <c r="H41" s="279" t="s">
+      <c r="H41" s="278" t="s">
         <v>37</v>
       </c>
       <c r="I41" s="107"/>
@@ -10336,11 +10370,11 @@
       <c r="M41" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="O41" s="303" t="str">
+      <c r="O41" s="302" t="str">
         <f>CONCATENATE(C46," ",C47," ",F46)</f>
         <v>Proximal Trachea and Bronchial Tree (max point dose)</v>
       </c>
-      <c r="P41" s="313">
+      <c r="P41" s="312">
         <f>G46</f>
         <v>1194</v>
       </c>
@@ -10371,11 +10405,11 @@
       <c r="M42" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="O42" s="303" t="str">
+      <c r="O42" s="302" t="str">
         <f>C48</f>
         <v>Dosimetrist:</v>
       </c>
-      <c r="P42" s="307" t="str">
+      <c r="P42" s="306" t="str">
         <f>C49</f>
         <v>??</v>
       </c>
@@ -10406,11 +10440,11 @@
       <c r="M43" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="O43" s="303" t="str">
+      <c r="O43" s="302" t="str">
         <f>G48</f>
         <v>Physicist:</v>
       </c>
-      <c r="P43" s="307" t="str">
+      <c r="P43" s="306" t="str">
         <f>G49</f>
         <v>??</v>
       </c>
@@ -10425,7 +10459,7 @@
       <c r="F44" s="98" t="s">
         <v>143</v>
       </c>
-      <c r="G44" s="341">
+      <c r="G44" s="334">
         <v>0</v>
       </c>
       <c r="H44" s="131"/>
@@ -10441,11 +10475,11 @@
       <c r="M44" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="O44" s="303" t="str">
+      <c r="O44" s="302" t="str">
         <f>J48</f>
         <v>Radiation Oncologist:</v>
       </c>
-      <c r="P44" s="307" t="str">
+      <c r="P44" s="306" t="str">
         <f>K49</f>
         <v>??</v>
       </c>
@@ -10453,16 +10487,16 @@
     <row r="45" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="94"/>
       <c r="C45" s="94"/>
-      <c r="D45" s="289" t="s">
+      <c r="D45" s="288" t="s">
         <v>129</v>
       </c>
-      <c r="E45" s="248" t="s">
+      <c r="E45" s="247" t="s">
         <v>37</v>
       </c>
-      <c r="F45" s="290" t="s">
+      <c r="F45" s="289" t="s">
         <v>121</v>
       </c>
-      <c r="G45" s="342">
+      <c r="G45" s="335">
         <v>0</v>
       </c>
       <c r="H45" s="146"/>
@@ -10476,20 +10510,20 @@
         <v>Yes</v>
       </c>
       <c r="M45" s="87"/>
-      <c r="O45" s="303" t="str">
+      <c r="O45" s="302" t="str">
         <f>B50</f>
         <v>NOTES:</v>
       </c>
-      <c r="P45" s="307">
+      <c r="P45" s="306">
         <f>C50</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="294" t="s">
+      <c r="A46" s="293" t="s">
         <v>209</v>
       </c>
-      <c r="B46" s="295" t="s">
+      <c r="B46" s="294" t="s">
         <v>210</v>
       </c>
       <c r="C46" s="151" t="s">
@@ -10519,13 +10553,13 @@
       <c r="M46" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="O46" s="300"/>
+      <c r="O46" s="299"/>
     </row>
     <row r="47" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="343">
+      <c r="A47" s="336">
         <v>10.4</v>
       </c>
-      <c r="B47" s="344">
+      <c r="B47" s="337">
         <v>1194</v>
       </c>
       <c r="C47" s="94" t="s">
@@ -10543,7 +10577,7 @@
       <c r="K47" s="128"/>
       <c r="L47" s="14"/>
       <c r="M47" s="87"/>
-      <c r="O47" s="300"/>
+      <c r="O47" s="299"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B48" s="94"/>
@@ -10564,7 +10598,7 @@
       <c r="K48" s="84"/>
       <c r="L48" s="86"/>
       <c r="M48" s="87"/>
-      <c r="O48" s="300"/>
+      <c r="O48" s="299"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B49" s="94"/>
@@ -10585,7 +10619,7 @@
       </c>
       <c r="L49" s="100"/>
       <c r="M49" s="87"/>
-      <c r="O49" s="300"/>
+      <c r="O49" s="299"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B50" s="101" t="s">
@@ -10602,26 +10636,26 @@
       <c r="K50" s="22"/>
       <c r="L50" s="17"/>
       <c r="M50" s="87"/>
-      <c r="O50" s="300"/>
+      <c r="O50" s="299"/>
     </row>
     <row r="51" spans="2:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B51" s="89"/>
       <c r="C51" s="90"/>
       <c r="D51" s="90"/>
       <c r="E51" s="90"/>
-      <c r="F51" s="256" t="s">
+      <c r="F51" s="255" t="s">
         <v>128</v>
       </c>
-      <c r="G51" s="257" t="s">
+      <c r="G51" s="256" t="s">
         <v>126</v>
       </c>
-      <c r="H51" s="256"/>
-      <c r="I51" s="257"/>
-      <c r="J51" s="257"/>
-      <c r="K51" s="256"/>
-      <c r="L51" s="258"/>
+      <c r="H51" s="255"/>
+      <c r="I51" s="256"/>
+      <c r="J51" s="256"/>
+      <c r="K51" s="255"/>
+      <c r="L51" s="257"/>
       <c r="M51" s="87"/>
-      <c r="O51" s="300"/>
+      <c r="O51" s="299"/>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B52" s="153" t="s">
@@ -10638,7 +10672,7 @@
       <c r="K52" s="154"/>
       <c r="L52" s="154"/>
       <c r="M52" s="87"/>
-      <c r="O52" s="300"/>
+      <c r="O52" s="299"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B53" s="88"/>
@@ -10653,7 +10687,7 @@
       <c r="K53" s="154"/>
       <c r="L53" s="154"/>
       <c r="M53" s="87"/>
-      <c r="O53" s="300"/>
+      <c r="O53" s="299"/>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F55" s="166"/>
@@ -12447,40 +12481,40 @@
       <c r="C27" s="69"/>
       <c r="D27" s="70"/>
       <c r="E27" s="71"/>
-      <c r="F27" s="70" t="e">
+      <c r="F27" s="70">
         <f ca="1">FORECAST(I30,OFFSET(F9:F19,MATCH(I30,D9:D19,1)-1,0,2),OFFSET(D9:D19,MATCH(I30,D9:D19,1)-1,0,2))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G27" s="70" t="e">
+        <v>1.2</v>
+      </c>
+      <c r="G27" s="70">
         <f ca="1">FORECAST(I30,OFFSET(G9:G19,MATCH(I30,D9:D19,1)-1,0,2),OFFSET(D9:D19,MATCH(I30,D9:D19,1)-1,0,2))</f>
-        <v>#VALUE!</v>
+        <v>1.5</v>
       </c>
       <c r="H27" s="71"/>
-      <c r="I27" s="70" t="e">
+      <c r="I27" s="70">
         <f ca="1">FORECAST(I30,OFFSET(I9:I19,MATCH(I30,D9:D19,1)-1,0,2),OFFSET(D9:D19,MATCH(I30,D9:D19,1)-1,0,2))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J27" s="70" t="e">
+        <v>4.2475000000000005</v>
+      </c>
+      <c r="J27" s="70">
         <f ca="1">FORECAST(I30,OFFSET(J9:J19,MATCH(I30,D9:D19,1)-1,0,2),OFFSET(D9:D19,MATCH(I30,D9:D19,1)-1,0,2))</f>
-        <v>#VALUE!</v>
+        <v>5.2475000000000005</v>
       </c>
       <c r="K27" s="71"/>
-      <c r="L27" s="70" t="e">
+      <c r="L27" s="70">
         <f ca="1">FORECAST(I30,OFFSET(L9:L19,MATCH(I30,D9:D19,1)-1,0,2),OFFSET(D9:D19,MATCH(I30,D9:D19,1)-1,0,2))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M27" s="70" t="e">
+        <v>58.7</v>
+      </c>
+      <c r="M27" s="70">
         <f ca="1">FORECAST(I30,OFFSET(M9:M19,MATCH(I30,D9:D19,1)-1,0,2),OFFSET(D9:D19,MATCH(I30,D9:D19,1)-1,0,2))</f>
-        <v>#VALUE!</v>
+        <v>69.575000000000003</v>
       </c>
       <c r="N27" s="71"/>
-      <c r="O27" s="70" t="e">
+      <c r="O27" s="70">
         <f ca="1">FORECAST(I30,OFFSET(O9:O19,MATCH(I30,D9:D19,1)-1,0,2),OFFSET(D9:D19,MATCH(I30,D9:D19,1)-1,0,2))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P27" s="70" t="e">
+        <v>10</v>
+      </c>
+      <c r="P27" s="70">
         <f ca="1">FORECAST(I30,OFFSET(P9:P19,MATCH(I30,D9:D19,1)-1,0,2),OFFSET(D9:D19,MATCH(I30,D9:D19,1)-1,0,2))</f>
-        <v>#VALUE!</v>
+        <v>15</v>
       </c>
       <c r="Q27" s="72"/>
     </row>
@@ -12535,9 +12569,9 @@
       <c r="H30" s="159" t="s">
         <v>108</v>
       </c>
-      <c r="I30" s="74" t="str">
+      <c r="I30" s="74">
         <f>'EvaluationSheet 60Gy 8F'!G9</f>
-        <v>??</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="J30" s="74"/>
       <c r="K30" s="61" t="s">
@@ -12559,17 +12593,17 @@
       <c r="H31" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="I31" s="74" t="str">
+      <c r="I31" s="74">
         <f>'EvaluationSheet 60Gy 8F'!G22</f>
-        <v>??</v>
-      </c>
-      <c r="J31" s="76" t="e">
+        <v>38.9</v>
+      </c>
+      <c r="J31" s="76">
         <f>I31/I30</f>
-        <v>#VALUE!</v>
+        <v>1.0570652173913044</v>
       </c>
       <c r="K31" s="74" t="str">
-        <f>IF(I31="??","??",IF(J31&lt;F27,F26,IF(J31&lt;=G27,G26,H26)))</f>
-        <v>??</v>
+        <f ca="1">IF(I31="??","??",IF(J31&lt;F27,F26,IF(J31&lt;=G27,G26,H26)))</f>
+        <v>Yes</v>
       </c>
       <c r="L31" s="61"/>
       <c r="M31" s="61"/>
@@ -12587,17 +12621,17 @@
       <c r="H32" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="I32" s="74" t="str">
+      <c r="I32" s="74">
         <f>'EvaluationSheet 60Gy 8F'!G25</f>
-        <v>??</v>
-      </c>
-      <c r="J32" s="76" t="e">
+        <v>161.5</v>
+      </c>
+      <c r="J32" s="76">
         <f>I32/I30</f>
-        <v>#VALUE!</v>
+        <v>4.3885869565217392</v>
       </c>
       <c r="K32" s="74" t="str">
-        <f>IF(I32="??", "??",IF(J32&lt;=I27,I26,IF(J32&lt;=J27,J26,K26)))</f>
-        <v>??</v>
+        <f ca="1">IF(I32="??", "??",IF(J32&lt;=I27,I26,IF(J32&lt;=J27,J26,K26)))</f>
+        <v>Minor Deviation</v>
       </c>
       <c r="L32" s="61"/>
       <c r="M32" s="61"/>
@@ -12615,17 +12649,17 @@
       <c r="H33" s="77" t="s">
         <v>118</v>
       </c>
-      <c r="I33" s="74" t="str">
+      <c r="I33" s="74">
         <f>'EvaluationSheet 60Gy 8F'!G24</f>
-        <v>??</v>
-      </c>
-      <c r="J33" s="76" t="str">
+        <v>54</v>
+      </c>
+      <c r="J33" s="76">
         <f>I33</f>
-        <v>??</v>
+        <v>54</v>
       </c>
       <c r="K33" s="74" t="str">
-        <f>IF(I33="??","??",IF(J33&lt;=L27,L26,IF(J33&lt;=M27,M26,N26)))</f>
-        <v>??</v>
+        <f ca="1">IF(I33="??","??",IF(J33&lt;=L27,L26,IF(J33&lt;=M27,M26,N26)))</f>
+        <v>Yes</v>
       </c>
       <c r="L33" s="61"/>
       <c r="M33" s="61"/>
@@ -12643,14 +12677,14 @@
       <c r="H34" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="I34" s="76" t="str">
+      <c r="I34" s="76">
         <f>'EvaluationSheet 60Gy 8F'!G31</f>
-        <v>??</v>
+        <v>5.5139066666666674E-2</v>
       </c>
       <c r="J34" s="74"/>
       <c r="K34" s="74" t="str">
         <f>IF(I34="??","??",IF(I34&lt;=0.1,O26,IF(I34&lt;=0.15,P26,Q26)))</f>
-        <v>??</v>
+        <v>Yes</v>
       </c>
       <c r="L34" s="61"/>
       <c r="M34" s="61"/>

</xml_diff>